<commit_message>
added score and stock analysis excel file
</commit_message>
<xml_diff>
--- a/aapl_sec_filings.xlsx
+++ b/aapl_sec_filings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\komendra sahu\Dropbox\PC\Desktop\DVA-sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60534ED0-73B3-4FDE-81DE-7BA8254106E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1551B1EA-131F-4FE9-AC90-43E0D1492DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,10 +160,10 @@
     <t>'Item 2. Management’s Discussion and Analysis of Financial Condition and Results of Operations This section and other parts of this Quarterly Report on Form 10‑Q contain forward-looking statements, within the meaning of the Private Securities Litigation Reform Act of 1995, that involve risks and uncertainties. Forward-looking statements provide current expectations of future events based on certain assumptions and include any statement that does not directly relate to any historical or current fact. Forward-looking statements can also be identified by words such as “future,” “anticipates,” “believes,” “estimates,” “expects,” “intends,” “plans,” “predicts,” “will,” “would,” “could,” “can,” “may,” and similar terms. Forward-looking statements are not guarantees of future performance and the Company’s actual results may differ significantly from the results discussed in the forward-looking statements. Factors that might cause such differences include, but are not limited to, those discussed in Part II, Item 1A of this Form 10-Q under the heading “Risk Factors,” which are incorporated herein by reference. The following discussion should be read in conjunction with the Company’s Annual Report on Form 10-K for the year ended September 24, 2016 (the “2016 Form 10-K”) filed with the U.S. Securities and Exchange Commission (the “SEC”) and the condensed consolidated financial statements and notes thereto included elsewhere in this Form 10-Q. All information presented herein is based on the Company’s fiscal calendar. Unless otherwise stated, references to particular years, quarters, months or periods refer to the Company’s fiscal years ended in September and the associated quarters, months and periods of those fiscal years. Each of the terms the “Company” and “Apple” as used herein refers collectively to Apple Inc. and its wholly-owned subsidiaries, unless otherwise stated. The Company assumes no obligation to revise or update any forward-looking statements for any reason, except as required by law. Available Information The Company’s Annual Report on Form 10-K, Quarterly Reports on Form 10-Q, Current Reports on Form 8-K, and amendments to reports filed pursuant to Sections 13(a) and 15(d) of the Securities Exchange Act of 1934, as amended (the “Exchange Act”), are filed with the SEC. The Company is subject to the informational requirements of the Exchange Act and files or furnishes reports, proxy statements, and other information with the SEC. Such reports and other information filed by the Company with the SEC are available free of charge on the Company’s website at investor.apple.com/sec.cfm when such reports are available on the SEC’s website. The public may read and copy any materials filed by the Company with the SEC at the SEC’s Public Reference Room at 100 F Street, NE, Room 1580, Washington, DC 20549. The public may obtain information on the operation of the Public Reference Room by calling the SEC at 1-800-SEC-0330. The SEC maintains an internet site that contains reports, proxy and information statements and other information regarding issuers that file electronically with the SEC at www.sec.gov. The contents of websites are not incorporated into this filing. Further, the Company’s references to website URLs are intended to be inactive textual references only. Overview and Highlights The Company designs, manufactures and markets mobile communication and media devices and personal computers, and sells a variety of related software, services, accessories, networking solutions and third-party digital content and applications. The Company’s products and services include iPhone®, iPad®, Mac®, Apple Watch®, Apple TV®, a portfolio of consumer and professional software applications, iOS, macOS®, watchOS® and tvOS™ operating systems, iCloud®, Apple Pay® and a variety of accessory, service and support offerings. The Company sells and delivers digital content and applications through the iTunes Store®, App Store®, Mac App Store, TV App Store, iBooks Store™ and Apple Music® (collectively “Digital Content and Services”). The Company sells its products worldwide through its retail stores, online stores and direct sales force, as well as through third-party cellular network carriers, wholesalers, retailers and value-added resellers. In addition, the Company sells a variety of third-party Apple-compatible products, including application software and various accessories through its retail and online stores. The Company sells to consumers, small and mid-sized businesses and education, enterprise and government customers. Business Strategy The Company is committed to bringing the best user experience to its customers through its innovative hardware, software and services. The Company’s business strategy leverages its unique ability to design and develop its own operating systems, hardware, application software and services to provide its customers products and solutions with innovative design, superior ease-of-use and seamless integration. As part of its strategy, the Company continues to expand its platform for the discovery and delivery of digital content and applications through its Digital Content and Services, which allows customers to discover and download digital content, iOS, Mac, Apple Watch and Apple TV applications, and books through either a Mac or Windows personal computer or through iPhone, iPad and iPod touch® devices (“iOS devices”), Apple TV and Apple Watch. The Company also supports a community for the development of third-party software and hardware products and digital content that complement the Company’s offerings. The Company believes a high-quality buying experience with knowledgeable salespersons who can convey the value of the Company’s products and services greatly enhances its ability to attract and retain customers. Therefore, the Company’s strategy also includes building and expanding its own retail and online stores and its third-party distribution network to effectively reach more customers and provide them with a high-quality sales and post-sales support experience. The Company believes ongoing investment in research and development (“R&amp;D”), marketing and advertising is critical to the development and sale of innovative products and technologies. 23 Business Seasonality and Product Introductions The Company has historically experienced higher net sales in its first quarter compared to other quarters in its fiscal year due in part to seasonal holiday demand. Additionally, new product introductions can significantly impact net sales, product costs and operating expenses. Product introductions can also impact the Company’s net sales to its indirect distribution channels as these channels are filled with new product inventory following a product introduction, and often, channel inventory of a particular product declines as the next related major product launch approaches. Net sales can also be affected when consumers and distributors anticipate a product introduction. However, neither historical seasonal patterns nor historical patterns of product introductions should be considered reliable indicators of the Company’s future pattern of product introductions, future net sales or financial performance. Fiscal Period The Company’s fiscal year is the 52 or 53-week period that ends on the last Saturday of September. The Company’s fiscal year 2017 will include 53 weeks and will end on September 30, 2017. A 14th week was included in the first quarter of 2017, as is done every five or six years, to realign the Company’s fiscal quarters with calendar quarters. Second Quarter Fiscal 2017 Highlights Net sales increased 5% or $2.3 billion during the second quarter of 2017 compared to the same quarter in 2016, primarily driven by strong growth in Services, Mac and Other Products, partially offset by the effect of weakness in foreign currencies relative to the U.S. dollar. Net sales reflected year-over-year growth in each of the geographic operating segments, with the exception of Greater China. During the second quarter of 2017, the Company introduced a new 9.7-inch iPad, which became available at the end of the quarter. The Company utilized $7.0 billion to repurchase shares of its common stock and paid dividends and dividend equivalents of $3.0 billion during the second quarter of 2017. Additionally, the Company issued $11.0 billion of U.S. dollar-denominated long-term debt. Sales Data The following table shows net sales by operating segment and net sales and unit sales by product for the three- and six-month periods ended April 1, 2017 and March 26, 2016 (dollars in millions and units in thousands): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 Change April 1, 2017 March 26, 2016 Change Net Sales by Operating Segment: Americas $ 21,157 $ 19,096 11 % $ 53,125 $ 48,421 10 % Europe 12,733 11,535 10 % 31,254 29,467 6 % Greater China 10,726 12,486 (14 )% 26,959 30,859 (13 )% Japan 4,485 4,281 5 % 10,251 9,075 13 % Rest of Asia Pacific 3,795 3,159 20 % 9,658 8,607 12 % Total net sales $ 52,896 $ 50,557 5 % $ 131,247 $ 126,429 4 % Net Sales by Product: iPhone (1) $ 33,249 $ 32,857 1 % $ 87,627 $ 84,492 4 % iPad (1) 3,889 4,413 (12 )% 9,422 11,497 (18 )% Mac (1) 5,844 5,107 14 % 13,088 11,853 10 % Services (2) 7,041 5,991 18 % 14,213 12,047 18 % Other Products (1)(3) 2,873 2,189 31 % 6,897 6,540 5 % Total net sales $ 52,896 $ 50,557 5 % $ 131,247 $ 126,429 4 % Unit Sales by Product: iPhone 50,763 51,193 (1 )% 129,053 125,972 2 % iPad 8,922 10,251 (13 )% 22,003 26,373 (17 )% Mac 4,199 4,034 4 % 9,573 9,346 2 % (1)Includes deferrals and amortization of related software upgrade rights and non-software services. (2)Includes revenue from Digital Content and Services, AppleCare®, Apple Pay, licensing and other services. (3)Includes sales of Apple TV, Apple Watch, Beats® products, iPod and Apple-branded and third-party accessories. 24 Product Performance iPhone The following table presents iPhone net sales and unit sales information for the three- and six-month periods ended April 1, 2017 and March 26, 2016 (dollars in millions and units in thousands): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 Change April 1, 2017 March 26, 2016 Change Net sales $ 33,249 $ 32,857 1 % $ 87,627 $ 84,492 4 % Percentage of total net sales 63 % 65 % 67 % 67 % Unit sales 50,763 51,193 (1 )% 129,053 125,972 2 % iPhone net sales increased during the second quarter of 2017 compared to the same period in 2016 due to higher iPhone average selling prices (“ASPs”), largely offset by the effect of weakness in foreign currencies relative to the U.S. dollar. The year-over-year increase in iPhone net sales during the first six months of 2017 was due primarily to higher iPhone unit sales and to a lesser extent higher iPhone ASPs, partially offset by the effect of weakness in foreign currencies relative to the U.S. dollar. iPad The following table presents iPad net sales and unit sales information for the three- and six-month periods ended April 1, 2017 and March 26, 2016 (dollars in millions and units in thousands): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 Change April 1, 2017 March 26, 2016 Change Net sales $ 3,889 $ 4,413 (12 )% $ 9,422 $ 11,497 (18 )% Percentage of total net sales 7 % 9 % 7 % 9 % Unit sales 8,922 10,251 (13 )% 22,003 26,373 (17 )% iPad net sales decreased in the second quarter and first six months of 2017 compared to the same periods in 2016 due primarily to lower iPad unit sales in each of the geographic operating segments and to a lesser extent the effect of weakness in foreign currencies relative to the U.S. dollar. Mac The following table presents Mac net sales and unit sales information for the three- and six-month periods ended April 1, 2017 and March 26, 2016 (dollars in millions and units in thousands): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 Change April 1, 2017 March 26, 2016 Change Net sales $ 5,844 $ 5,107 14 % $ 13,088 $ 11,853 10 % Percentage of total net sales 11 % 10 % 10 % 9 % Unit sales 4,199 4,034 4 % 9,573 9,346 2 % Mac net sales increased during the second quarter and first six months of 2017 compared to the same periods in 2016 due primarily to a different mix of Macs, including the new MacBook Pro introduced in the first quarter of 2017, and to a lesser extent higher Mac unit sales. The year-over-year increase in Mac net sales was partially offset by the effect of weakness in foreign currencies relative to the U.S. dollar. 25 Services The following table presents Services net sales information for the three- and six-month periods ended April 1, 2017 and March 26, 2016 (dollars in millions): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 Change April 1, 2017 March 26, 2016 Change Net sales $ 7,041 $ 5,991 18 % $ 14,213 $ 12,047 18 % Percentage of total net sales 13 % 12 % 11 % 10 % The year-over-year increase in Services net sales in the second quarter and first six months of 2017 compared to the same periods in 2016 was due primarily to growth from the App Store and licensing sales. The year-over-year increase in Services net sales during the first six months of 2017 was partially offset by the non-recurrence of the $548 million received from Samsung Electronics Co., Ltd. in the first quarter of 2016 related to patent infringement matters. Segment Operating Performance The Company manages its business primarily on a geographic basis. The Company’s reportable operating segments consist of the Americas, Europe, Greater China, Japan and Rest of Asia Pacific. The Americas segment includes both North and South America. The Europe segment includes European countries, as well as India, the Middle East and Africa. The Greater China segment includes China, Hong Kong and Taiwan. The Rest of Asia Pacific segment includes Australia and those Asian countries not included in the Company’s other reportable operating segments. Although the reportable operating segments provide similar hardware and software products and similar services, each one is managed separately to better align with the location of the Company’s customers and distribution partners and the unique market dynamics of each geographic region. Further information regarding the Company’s reportable operating segments can be found in Part I, Item 1 of this Form 10-Q in the Notes to Condensed Consolidated Financial Statements, in Note 11, “Segment Information and Geographic Data.” Americas The following table presents Americas net sales information for the three- and six-month periods ended April 1, 2017 and March 26, 2016 (dollars in millions): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 Change April 1, 2017 March 26, 2016 Change Net sales $ 21,157 $ 19,096 11 % $ 53,125 $ 48,421 10 % Percentage of total net sales 40 % 38 % 40 % 38 % Americas net sales increased during the second quarter of 2017 compared to the same period in 2016 due primarily to higher net sales of iPhone and Other Products. The year-over-year increase in Americas net sales during the first six months of 2017 was due primarily to higher net sales of iPhone and Mac, partially offset by lower net sales of iPad. Europe The following table presents Europe net sales information for the three- and six-month periods ended April 1, 2017 and March 26, 2016 (dollars in millions): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 Change April 1, 2017 March 26, 2016 Change Net sales $ 12,733 $ 11,535 10 % $ 31,254 $ 29,467 6 % Percentage of total net sales 24 % 23 % 24 % 23 % Europe net sales increased during the second quarter of 2017 compared to the same period in 2016 due primarily to higher net sales of iPhone and Mac, partially offset by the effect of weakness in foreign currencies relative to the U.S. dollar. The year-over-year increase in Europe net sales during the first six months of 2017 was due primarily to higher net sales of iPhone and Services, partially offset by the effect of weakness in foreign currencies relative to the U.S. dollar and to a lesser extent lower net sales of iPad. 26 Greater China The following table presents Greater China net sales information for the three- and six-month periods ended April 1, 2017 and March 26, 2016 (dollars in millions): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 Change April 1, 2017 March 26, 2016 Change Net sales $ 10,726 $ 12,486 (14 )% $ 26,959 $ 30,859 (13 )% Percentage of total net sales 20 % 25 % 21 % 24 % Greater China net sales decreased during the second quarter and first six months of 2017 compared to the same periods in 2016 due primarily to lower net sales of iPhone and the effect of weakness in foreign currencies relative to the U.S. dollar, partially offset by growth in net sales of Services. Japan The following table presents Japan net sales information for the three- and six-month periods ended April 1, 2017 and March 26, 2016 (dollars in millions): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 Change April 1, 2017 March 26, 2016 Change Net sales $ 4,485 $ 4,281 5 % $ 10,251 $ 9,075 13 % Percentage of total net sales 8 % 8 % 8 % 7 % Japan net sales increased during the second quarter of 2017 compared to the same period in 2016 due primarily to higher net sales of Services and the effect of strength in the Japanese yen relative to the U.S. dollar. The year-over-year increase in Japan net sales during the first six months of 2017 was due primarily to the effect of strength in the Japanese yen relative to the U.S. dollar and growth in net sales of iPhone. Rest of Asia Pacific The following table presents Rest of Asia Pacific net sales information for the three- and six-month periods ended April 1, 2017 and March 26, 2016 (dollars in millions): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 Change April 1, 2017 March 26, 2016 Change Net sales $ 3,795 $ 3,159 20 % $ 9,658 $ 8,607 12 % Percentage of total net sales 7 % 6 % 7 % 7 % Rest of Asia Pacific net sales increased during the second quarter of 2017 compared to the same period in 2016 due primarily to higher net sales of iPhone and Mac. The year-over-year increase in Rest of Asia Pacific net sales during the first six months of 2017 was due primarily to higher net sales of iPhone and the effect of strength in foreign currencies relative to the U.S. dollar. Gross Margin Gross margin for the three- and six-month periods ended April 1, 2017 and March 26, 2016 was as follows (dollars in millions): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 April 1, 2017 March 26, 2016 Net sales $ 52,896 $ 50,557 $ 131,247 $ 126,429 Cost of sales 32,305 30,636 80,480 76,085 Gross margin $ 20,591 $ 19,921 $ 50,767 $ 50,344 Gross margin percentage 38.9 % 39.4 % 38.7 % 39.8 % Gross margin decreased during the second quarter and first six months of 2017 compared to the same periods in 2016 due primarily to higher product cost structures and the effect of weakness in foreign currencies relative to the U.S. dollar, partially offset by a favorable mix of products and services. 27 The Company anticipates gross margin during the third quarter of 2017 to be between 37.5% and 38.5%. The foregoing statement regarding the Company’s expected gross margin percentage in the third quarter of 2017 is forward-looking and could differ from actual results. The Company’s future gross margins can be impacted by multiple factors including, but not limited to, those set forth in Part II, Item 1A of this Form 10-Q under the heading “Risk Factors” and those described in this paragraph. In general, the Company believes gross margins will remain under downward pressure due to a variety of factors, including continued industry-wide global product pricing pressures, increased competition, compressed product life cycles, product transitions, potential increases in the cost of components, and potential strengthening of the U.S. dollar, as well as potential increases in the costs of outside manufacturing services and a potential shift in the Company’s sales mix towards products with lower gross margins. In response to competitive pressures, the Company expects it will continue to take product pricing actions, which would adversely affect gross margins. Gross margins could also be affected by the Company’s ability to manage product quality and warranty costs effectively and to stimulate demand for certain of its products. Due to the Company’s significant international operations, its financial condition and operating results, including gross margins, could be significantly affected by fluctuations in exchange rates. Operating Expenses Operating expenses for the three- and six-month periods ended April 1, 2017 and March 26, 2016 were as follows (dollars in millions): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 April 1, 2017 March 26, 2016 Research and development $ 2,776 $ 2,511 $ 5,647 $ 4,915 Percentage of total net sales 5 % 5 % 4 % 4 % Selling, general and administrative $ 3,718 $ 3,423 $ 7,664 $ 7,271 Percentage of total net sales 7 % 7 % 6 % 6 % Total operating expenses $ 6,494 $ 5,934 $ 13,311 $ 12,186 Percentage of total net sales 12 % 12 % 10 % 10 % Research and Development The growth in R&amp;D expense during the second quarter and first six months of 2017 compared to the same periods in 2016 was driven primarily by an increase in headcount and related expenses to support expanded R&amp;D activities. The Company continues to believe that focused investments in R&amp;D are critical to its future growth and competitive position in the marketplace, and to the development of new and updated products that are central to the Company’s core business strategy. Selling, General and Administrative The growth in selling, general and administrative expense during the second quarter of 2017 compared to the same quarter in 2016 was driven primarily by an increase in headcount and related expenses and higher spending on marketing and advertising. The year-over-year growth in selling, general and administrative expense during the first six months of 2017 was driven primarily by an increase in headcount and related expenses and higher variable selling costs. Other Income/(Expense), Net Other income/(expense), net for the three- and six-month periods ended April 1, 2017 and March 26, 2016 was as follows (dollars in millions): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 Change April 1, 2017 March 26, 2016 Change Interest and dividend income $ 1,282 $ 986 $ 2,506 $ 1,927 Interest expense (530 ) (321 ) (1,055 ) (597 ) Other expense, net (165 ) (510 ) (43 ) (773 ) Total other income/(expense), net $ 587 $ 155 279 % $ 1,408 $ 557 153 % The increase in other income/(expense), net during the second quarter and first six months of 2017 compared to the same periods in 2016 was due primarily to higher interest income and the favorable impact of foreign exchange-related items, partially offset by higher interest expense on debt. The weighted-average interest rate earned by the Company on its cash, cash equivalents and marketable securities was 1.99% and 1.74% in the second quarter of 2017 and 2016, respectively, and 1.93% and 1.70% in the first six months of 2017 and 2016, respectively. Provision for Income Taxes Provision for income taxes and effective tax rates for the three- and six-month periods ended April 1, 2017 and March 26, 2016 were as follows (dollars in millions): Three Months Ended Six Months Ended April 1, 2017 March 26, 2016 April 1, 2017 March 26, 2016 Provision for income taxes $ 3,655 $ 3,626 $ 9,944 $ 9,838 Effective tax rate 24.9 % 25.6 % 25.6 % 25.4 % The Company’s effective tax rates during the second quarter of 2017 and 2016 differ from the statutory federal income tax rate of 35% due primarily to certain undistributed foreign earnings, a substantial portion of which was generated by subsidiaries organized in Ireland, for which no U.S. taxes are provided when such earnings are intended to be indefinitely reinvested outside the U.S. The lower effective tax rate during the second quarter of 2017 compared to the same quarter in 2016 was due primarily to a different geographic mix of earnings. The slightly higher effective tax rate in the first six months of 2017 compared to the same period in 2016 was due primarily to the retroactive reinstatement of the U.S. federal R&amp;D tax credit during the first quarter of 2016. The Company is subject to audits by federal, state, local and foreign tax authorities. Management believes that adequate provisions have been made for any adjustments that may result from tax examinations. However, the outcome of tax audits cannot be predicted with certainty. If any issues addressed in the Company’s tax audits are resolved in a manner not consistent with management’s expectations, the Company could be required to adjust its provision for income taxes in the period such resolution occurs. On August 30, 2016, the European Commission announced its decision that Ireland granted state aid to the Company by providing tax opinions in 1991 and 2007 concerning the tax allocation of profits of the Irish branches of two subsidiaries of the Company (the “State Aid Decision”). The State Aid Decision orders Ireland to calculate and recover additional taxes from the Company for the period June 2003 through December 2014. Irish legislative changes, effective as of January 2015, eliminated the application of the tax opinions from that date forward. The Company believes the State Aid Decision to be without merit and appealed to the General Court of the Court of Justice of the European Union. Ireland has also appealed the State Aid Decision. While the European Commission announced a recovery amount of up to €13 billion, plus interest, the actual amount of additional taxes subject to recovery is to be calculated by Ireland in accordance with the European Commission's guidance. Once the recovery amount is computed by Ireland, the Company anticipates funding it, including interest, out of foreign cash into escrow, where it will remain pending conclusion of all appeals. The Company believes that any incremental Irish corporate income taxes potentially due related to the State Aid Decision would be creditable against U.S. taxes. Recent Accounting Pronouncements Restricted Cash In November 2016, the Financial Accounting Standards Board (“FASB”) issued Accounting Standards Update (“ASU”) No. 2016-18, Statement of Cash Flows (Topic 230): Restricted Cash (“ASU 2016-18”), which enhances and clarifies the guidance on the classification and presentation of restricted cash in the statement of cash flows. The Company will adopt ASU 2016-18 in its first quarter of 2019 utilizing the retrospective adoption method. Currently, the Company's restricted cash balance is not significant. Income Taxes In October 2016, the FASB issued ASU No. 2016-16, Income Taxes (Topic 740): Intra-Entity Transfers of Assets Other Than Inventory (“ASU 2016-16”), which requires the recognition of the income tax consequences of an intra-entity transfer of an asset, other than inventory, when the transfer occurs. The Company will adopt ASU 2016-16 in its first quarter of 2019 utilizing the modified retrospective adoption method. Currently, the Company anticipates recording up to $9 billion of net deferred tax assets on its Consolidated Balance Sheets. However, the ultimate impact of adopting ASU 2016-16 will depend on the balance of intellectual property transferred between its subsidiaries as of the adoption date. The Company will recognize incremental deferred income tax expense thereafter as these deferred tax assets are utilized. Stock Compensation In March 2016, the FASB issued ASU No. 2016-09, Compensation – Stock Compensation (Topic 718): Improvements to Employee Share-Based Payment Accounting (“ASU 2016-09”), which modifies certain aspects of the accounting for share-based payment transactions, including income taxes, classification of awards, and classification in the statement of cash flows. The Company will adopt ASU 2016-09 in its first quarter of 2018. Currently, excess tax benefits or deficiencies from the Company's equity awards are recorded as additional paid-in capital in its Consolidated Balance Sheets. Upon adoption, the Company will record any excess tax benefits or deficiencies from its equity awards in its Consolidated Statements of Operations in the reporting periods in which vesting occurs. As a result, subsequent to adoption the Company's income tax expense and associated effective tax rate will be impacted by fluctuations in stock price between the grant dates and vesting dates of equity awards. 28 Leases In February 2016, the FASB issued ASU No. 2016-02, Leases (Topic 842) (“ASU 2016-02”), which modifies lease accounting for lessees to increase transparency and comparability by recording lease assets and liabilities for operating leases and disclosing key information about leasing arrangements. ASU 2016-02 will be effective for the Company beginning in its first quarter of 2020, and early adoption is permitted. The Company will use a modified retrospective adoption approach. While the Company is currently evaluating the timing and impact of adopting ASU 2016-02, currently the Company anticipates recording lease assets and liabilities in excess of $8.2 billion on its Consolidated Balance Sheets, with no material impact to its Consolidated Statements of Operations. However, the ultimate impact of adopting ASU 2016-02 will depend on the Company's lease portfolio as of the adoption date. Financial Instruments In January 2016, the FASB issued ASU No. 2016-01, Financial Instruments – Overall (Subtopic 825-10): Recognition and Measurement of Financial Assets and Financial Liabilities (“ASU 2016-01”), which updates certain aspects of recognition, measurement, presentation and disclosure of financial instruments. The Company will adopt ASU 2016-01 in its first quarter of 2019 utilizing the modified retrospective adoption method. Based on the composition of the Company's investment portfolio, the adoption of ASU 2016-01 is not expected to have a material impact on its consolidated financial statements. In June 2016, the FASB issued ASU No. 2016-13, Financial Instruments – Credit Losses (Topic 326): Measurement of Credit Losses on Financial Instruments (“ASU 2016-13”), which modifies the measurement of expected credit losses of certain financial instruments. The Company will adopt ASU 2016-13 in its first quarter of 2021 utilizing the modified retrospective adoption method. Based on the composition of the Company's investment portfolio, current market conditions, and historical credit loss activity, the adoption of ASU 2016-13 is not expected to have a material impact on its consolidated financial statements. Revenue Recognition In May 2014, the FASB issued ASU No. 2014-09, Revenue from Contracts with Customers (Topic 606) (“ASU 2014-09”), which amends the existing accounting standards for revenue recognition. ASU 2014-09 is based on principles that govern the recognition of revenue at an amount an entity expects to be entitled when products are transferred to customers. Subsequently, the FASB has issued the following standards related to ASU 2014-09: ASU No. 2016-08, Revenue from Contracts with Customers (Topic 606): Principal versus Agent Considerations (“ASU 2016-08”); ASU No. 2016-10, Revenue from Contracts with Customers (Topic 606): Identifying Performance Obligations and Licensing (“ASU 2016-10”); ASU No. 2016-12, Revenue from Contracts with Customers (Topic 606): Narrow-Scope Improvements and Practical Expedients (“ASU 2016-12”); and ASU No. 2016-20, Technical Corrections and Improvements to Topic 606, Revenue from Contracts with Customers (“ASU 2016-20”). The Company must adopt ASU 2016-08, ASU 2016-10, ASU 2016-12 and ASU 2016-20 with ASU 2014-09 (collectively, the “new revenue standards”). The new revenue standards may be applied retrospectively to each prior period presented or retrospectively with the cumulative effect recognized as of the date of adoption. The Company plans to adopt the new revenue standards in its first quarter of 2019 utilizing the full retrospective adoption method. The new revenue standards are not expected to have a material impact on the amount and timing of revenue recognized in the Company's consolidated financial statements. Liquidity and Capital Resources The following tables present selected financial information and statistics as of April 1, 2017 and September 24, 2016 and for the first six months of 2017 and 2016 (in millions): April 1, 2017 September 24, 2016 Cash, cash equivalents and market</t>
   </si>
   <si>
-    <t>'Item 2. Management’s Discussion and Analysis of Financial Condition and Results of Operations This section and other parts of this Quarterly Report on Form 10‑Q contain forward-looking statements, within the meaning of the Private Securities Litigation Reform Act of 1995, that involve risks and uncertainties. Forward-looking statements provide current expectations of future events based on certain assumptions and include any statement that does not directly relate to any historical or current fact. Forward-looking statements can also be identified by words such as “future,” “anticipates,” “believes,” “estimates,” “expects,” “intends,” “plans,” “predicts,” “will,” “would,” “could,” “can,” “may,” and similar terms. Forward-looking statements are not guarantees of future performance and the Company’s actual results may differ significantly from the results discussed in the forward-looking statements. Factors that might cause such differences include, but are not limited to, those discussed in Part II, Item 1A of this Form 10-Q under the heading “Risk Factors,” which are incorporated herein by reference. The following discussion should be read in conjunction with the Company’s Annual Report on Form 10-K for the year ended September 24, 2016 (the “2016 Form 10-K”) filed with the U.S. Securities and Exchange Commission (the “SEC”) and the condensed consolidated financial statements and notes thereto included elsewhere in this Form 10-Q. All information presented herein is based on the Company’s fiscal calendar. Unless otherwise stated, references to particular years, quarters, months or periods refer to the Company’s fiscal years ended in September and the associated quarters, months and periods of those fiscal years. Each of the terms the “Company” and “Apple” as used herein refers collectively to Apple Inc. and its wholly-owned subsidiaries, unless otherwise stated. The Company assumes no obligation to revise or update any forward-looking statements for any reason, except as required by law. Available Information The Company’s Annual Report on Form 10-K, Quarterly Reports on Form 10-Q, Current Reports on Form 8-K, and amendments to reports filed pursuant to Sections 13(a) and 15(d) of the Securities Exchange Act of 1934, as amended (the “Exchange Act”), are filed with the SEC. The Company is subject to the informational requirements of the Exchange Act and files or furnishes reports, proxy statements, and other information with the SEC. Such reports and other information filed by the Company with the SEC are available free of charge on the Company’s website at investor.apple.com/sec.cfm when such reports are available on the SEC’s website. The public may read and copy any materials filed by the Company with the SEC at the SEC’s Public Reference Room at 100 F Street, NE, Room 1580, Washington, DC 20549. The public may obtain information on the operation of the Public Reference Room by calling the SEC at 1-800-SEC-0330. The SEC maintains an internet site that contains reports, proxy and information statements and other information regarding issuers that file electronically with the SEC at www.sec.gov. The contents of websites are not incorporated into this filing. Further, the Company’s references to website URLs are intended to be inactive textual references only. Overview and Highlights The Company designs, manufactures and markets mobile communication and media devices, personal computers and portable digital music players, and sells a variety of related software, services, accessories, networking solutions and third-party digital content and applications. The Company’s products and services include iPhone®, iPad®, Mac®, iPod®, Apple Watch®, Apple TV®, a portfolio of consumer and professional software applications, iOS, macOS™, watchOS® and tvOS™ operating systems, iCloud®, Apple Pay® and a variety of accessory, service and support offerings. The Company sells and delivers digital content and applications through the iTunes Store®, App Store®, Mac App Store, TV App Store, iBooks Store™ and Apple Music® (collectively “Digital Content and Services”). The Company sells its products worldwide through its retail stores, online stores and direct sales force, as well as through third-party cellular network carriers, wholesalers, retailers and value-added resellers. In addition, the Company sells a variety of third-party Apple-compatible products, including application software and various accessories through its retail and online stores. The Company sells to consumers, small and mid-sized businesses and education, enterprise and government customers. Business Strategy The Company is committed to bringing the best user experience to its customers through its innovative hardware, software and services. The Company’s business strategy leverages its unique ability to design and develop its own operating systems, hardware, application software and services to provide its customers products and solutions with innovative design, superior ease-of-use and seamless integration. As part of its strategy, the Company continues to expand its platform for the discovery and delivery of digital content and applications through its Digital Content and Services, which allows customers to discover and download digital content, iOS, Mac, Apple Watch and Apple TV applications, and books through either a Mac or Windows personal computer or through iPhone, iPad and iPod touch® devices (“iOS devices”), Apple TV and Apple Watch. The Company also supports a community for the development of third-party software and hardware products and digital content that complement the Company’s offerings. The Company believes a high-quality buying experience with knowledgeable salespersons who can convey the value of the Company’s products and services greatly enhances its ability to attract and retain customers. Therefore, the Company’s strategy also includes building and expanding its own retail and online stores and its third-party distribution network to effectively reach more customers and provide them with a high-quality sales and post-sales support experience. The Company believes ongoing investment in research and development (“R&amp;D”), marketing and advertising is critical to the development and sale of innovative products and technologies. 22 Business Seasonality and Product Introductions The Company has historically experienced higher net sales in its first quarter compared to other quarters in its fiscal year due in part to seasonal holiday demand. Additionally, new product introductions can significantly impact net sales, product costs and operating expenses. Product introductions can also impact the Company’s net sales to its indirect distribution channels as these channels are filled with new product inventory following a product introduction, and often, channel inventory of a particular product declines as the next related major product launch approaches. Net sales can also be affected when consumers and distributors anticipate a product introduction. However, neither historical seasonal patterns nor historical patterns of product introductions should be considered reliable indicators of the Company’s future pattern of product introductions, future net sales or financial performance. Fiscal Period The Company’s fiscal year is the 52 or 53-week period that ends on the last Saturday of September. The Company’s fiscal year 2017 will include 53 weeks and will end on September 30, 2017. A 14th week has been included in the first quarter of 2017, as is done every five or six years, to realign the Company’s fiscal quarters with calendar quarters. First Quarter Fiscal 2017 Highlights Net sales grew 3% or $2.5 billion during the first quarter of 2017 compared to the first quarter of 2016, primarily driven by strong growth in iPhone and Services, partially offset by lower iPad sales. The positive impact of having an additional week in the first quarter of 2017 was primarily offset by lower year-over-year channel inventory growth, an earlier launch of iPhone 7 and 7 Plus as compared to the prior year and the effect of weakness in foreign currencies relative to the U.S. dollar. During the first quarter of 2017, the Company introduced a new MacBook Pro® with Touch Bar™, an interface that replaces the traditional row of function keys, and released AirPods™, which are new wireless headphones. Sales Data The following table shows net sales by operating segment and net sales and unit sales by product for the three months ended December 31, 2016 and December 26, 2015 (dollars in millions and units in thousands): Three Months Ended December 31, 2016 December 26, 2015 Change Net Sales by Operating Segment: Americas $ 31,968 $ 29,325 9 % Europe 18,521 17,932 3 % Greater China 16,233 18,373 (12 )% Japan 5,766 4,794 20 % Rest of Asia Pacific 5,863 5,448 8 % Total net sales $ 78,351 $ 75,872 3 % Net Sales by Product: iPhone (1) $ 54,378 $ 51,635 5 % iPad (1) 5,533 7,084 (22 )% Mac (1) 7,244 6,746 7 % Services (2) 7,172 6,056 18 % Other Products (1)(3) 4,024 4,351 (8 )% Total net sales $ 78,351 $ 75,872 3 % Unit Sales by Product: iPhone 78,290 74,779 5 % iPad 13,081 16,122 (19 )% Mac 5,374 5,312 1 % (1) Includes deferrals and amortization of related software upgrade rights and non-software services. (2) Includes revenue from Digital Content and Services, AppleCare®, Apple Pay, licensing and other services. (3) Includes sales of Apple TV, Apple Watch, Beats® products, iPod and Apple-branded and third-party accessories. 23 Product Performance iPhone The following table presents iPhone net sales and unit sales information for the first quarter of 2017 and 2016 (dollars in millions and units in thousands): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 54,378 $ 51,635 5 % Percentage of total net sales 69 % 68 % Unit sales 78,290 74,779 5 % iPhone net sales increased during the first quarter of 2017 compared to the same quarter in 2016, driven by strong growth in each of the geographic operating segments, with the exception of Greater China. iPad The following table presents iPad net sales and unit sales information for the first quarter of 2017 and 2016 (dollars in millions and units in thousands): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 5,533 $ 7,084 (22 )% Percentage of total net sales 7 % 9 % Unit sales 13,081 16,122 (19 )% iPad net sales decreased in the first quarter of 2017 compared to the same quarter in 2016 due to lower iPad unit sales and lower average selling prices for iPad, both due in part to the introduction of the 12.9-inch iPad Pro in the first quarter of 2016. Mac The following table presents Mac net sales and unit sales information for the first quarter of 2017 and 2016 (dollars in millions and units in thousands): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 7,244 $ 6,746 7 % Percentage of total net sales 9 % 9 % Unit sales 5,374 5,312 1 % Mac net sales increased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to a different mix of Macs, including the new MacBook Pro introduced in the first quarter of 2017. Services The following table presents Services net sales information for the first quarter of 2017 and 2016 (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 7,172 $ 6,056 18 % Percentage of total net sales 9 % 8 % The year-over-year increase in Services net sales in the first quarter of 2017 compared to the same quarter in 2016 was due primarily to growth from the App Store and AppleCare sales, partially offset by the $548 million received from Samsung Electronics Co., Ltd. in the first quarter of 2016 related to patent infringement matters. 24 Segment Operating Performance The Company manages its business primarily on a geographic basis. The Company’s reportable operating segments consist of the Americas, Europe, Greater China, Japan and Rest of Asia Pacific. The Americas segment includes both North and South America. The Europe segment includes European countries, as well as India, the Middle East and Africa. The Greater China segment includes China, Hong Kong and Taiwan. The Rest of Asia Pacific segment includes Australia and those Asian countries not included in the Company’s other reportable operating segments. Although the reportable operating segments provide similar hardware and software products and similar services, each one is managed separately to better align with the location of the Company’s customers and distribution partners and the unique market dynamics of each geographic region. Further information regarding the Company’s reportable operating segments can be found in Part I, Item 1 of this Form 10-Q in the Notes to Condensed Consolidated Financial Statements, in Note 11, “Segment Information and Geographic Data.” Americas The following table presents Americas net sales information for the first quarter of 2017 and 2016 (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 31,968 $ 29,325 9 % Percentage of total net sales 41 % 39 % Americas net sales increased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to higher net sales of iPhone, partially offset by lower net sales of iPad. Europe The following table presents Europe net sales information for the first quarter of 2017 and 2016 (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 18,521 $ 17,932 3 % Percentage of total net sales 24 % 24 % Europe net sales increased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to higher net sales of iPhone, partially offset by the effect of weakness in foreign currencies relative to the U.S. dollar and a decrease in net sales of iPad. Greater China The following table presents Greater China net sales information for the first quarter of 2017 and 2016 (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 16,233 $ 18,373 (12 )% Percentage of total net sales 21 % 24 % Greater China net sales decreased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to lower net sales of iPhone and the effect of weakness in foreign currencies relative to the U.S. dollar. 25 Japan The following table presents Japan net sales information for the first quarter of 2017 and 2016 (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 5,766 $ 4,794 20 % Percentage of total net sales 7 % 6 % Japan net sales increased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to higher net sales of iPhone and Services, and the effect of strength in the Japanese yen relative to the U.S. dollar. Rest of Asia Pacific The following table presents Rest of Asia Pacific net sales information for the first quarter of 2017 and 2016 (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 5,863 $ 5,448 8 % Percentage of total net sales 7 % 7 % Rest of Asia Pacific net sales increased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to higher net sales of iPhone and the effect of strength in foreign currencies relative to the U.S. dollar. Gross Margin Gross margin for the first quarter of 2017 and 2016 was as follows (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Net sales $ 78,351 $ 75,872 Cost of sales 48,175 45,449 Gross margin $ 30,176 $ 30,423 Gross margin percentage 38.5 % 40.1 % Gross margin decreased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to higher product cost structures and the effect of weakness in foreign currencies relative to the U.S. dollar, partially offset by a favorable mix of products and services. The Company anticipates gross margin during the second quarter of 2017 to be between 38% and 39%. The foregoing statement regarding the Company’s expected gross margin percentage in the second quarter of 2017 is forward-looking and could differ from actual results. The Company’s future gross margins can be impacted by multiple factors including, but not limited to, those set forth in Part II, Item 1A of this Form 10-Q under the heading “Risk Factors” and those described in this paragraph. In general, the Company believes gross margins will remain under downward pressure due to a variety of factors, including continued industry-wide global product pricing pressures, increased competition, compressed product life cycles, product transitions, potential increases in the cost of components, and potential strengthening of the U.S. dollar, as well as potential increases in the costs of outside manufacturing services and a potential shift in the Company’s sales mix towards products with lower gross margins. In response to competitive pressures, the Company expects it will continue to take product pricing actions, which would adversely affect gross margins. Gross margins could also be affected by the Company’s ability to manage product quality and warranty costs effectively and to stimulate demand for certain of its products. Due to the Company’s significant international operations, its financial condition and operating results, including gross margins, could be significantly affected by fluctuations in exchange rates. 26 Operating Expenses Operating expenses for the first quarter of 2017 and 2016 were as follows (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Research and development $ 2,871 $ 2,404 Percentage of total net sales 4 % 3 % Selling, general and administrative $ 3,946 $ 3,848 Percentage of total net sales 5 % 5 % Total operating expenses $ 6,817 $ 6,252 Percentage of total net sales 9 % 8 % Research and Development The growth in R&amp;D expense during the first quarter of 2017 compared to the same quarter in 2016 was driven primarily by an increase in headcount and related expenses, and material costs to support expanded R&amp;D activities. The Company continues to believe that focused investments in R&amp;D are critical to its future growth and competitive position in the marketplace, and to the development of new and updated products that are central to the Company’s core business strategy. Selling, General and Administrative The growth in selling, general and administrative expense during the first quarter of 2017 compared to the same quarter in 2016 was driven primarily by an increase in headcount and related expenses and higher variable selling costs, partially offset by lower advertising costs. Other Income/(Expense), Net Other income/(expense), net for the first quarter of 2017 and 2016 was as follows (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Interest and dividend income $ 1,224 $ 941 Interest expense (525 ) (276 ) Other income/(expense), net 122 (263 ) Total other income/(expense), net $ 821 $ 402 104 % The increase in other income/(expense), net during the first quarter of 2017 compared to the same quarter in 2016 was due primarily to higher interest income and foreign exchange gains, partially offset by higher interest expense on debt. The weighted-average interest rate earned by the Company on its cash, cash equivalents and marketable securities was 1.87% and 1.65% in the first quarter of 2017 and 2016, respectively. Provision for Income Taxes Provision for income taxes and effective tax rates for the first quarter of 2017 and 2016 were as follows (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Provision for income taxes $ 6,289 $ 6,212 Effective tax rate 26.0 % 25.3 % The Company’s effective tax rates during the first quarter of 2017 and 2016 differ from the statutory federal income tax rate of 35% due primarily to certain undistributed foreign earnings, a substantial portion of which was generated by subsidiaries organized in Ireland, for which no U.S. taxes are provided when such earnings are intended to be indefinitely reinvested outside the U.S. The higher year-over-year effective tax rate during the first quarter of 2017 was due primarily to the retroactive reinstatement of the U.S. federal R&amp;D tax credit during the first quarter of 2016. 27 The Company is subject to audits by federal, state, local and foreign tax authorities. Management believes that adequate provisions have been made for any adjustments that may result from tax examinations. However, the outcome of tax audits cannot be predicted with certainty. If any issues addressed in the Company’s tax audits are resolved in a manner not consistent with management’s expectations, the Company could be required to adjust its provision for income taxes in the period such resolution occurs. On August 30, 2016, the European Commission announced its decision that Ireland granted state aid to the Company by providing tax opinions in 1991 and 2007 concerning the tax allocation of profits of the Irish branches of two subsidiaries of the Company (the “State Aid Decision”). The State Aid Decision orders Ireland to calculate and recover additional taxes from the Company for the period June 2003 through December 2014. Irish legislative changes, effective as of January 2015, eliminated the application of the tax opinions from that date forward. The Company believes the State Aid Decision to be without merit and appealed to the General Court of the Court of Justice of the European Union. Ireland has also appealed the State Aid Decision. While the European Commission announced a recovery amount of up to €13 billion, plus interest, the actual amount of additional taxes subject to recovery is to be calculated by Ireland in accordance with the European Commission's guidance. Once the recovery amount is computed by Ireland, the Company anticipates funding it, including interest, out of foreign cash into escrow, where it will remain pending conclusion of all appeals. The Company believes that any incremental Irish corporate income taxes potentially due related to the State Aid Decision would be creditable against U.S. taxes. Recent Accounting Pronouncements Restricted Cash In November 2016, the Financial Accounting Standards Board (“FASB”) issued Accounting Standards Update (“ASU”) No. 2016-18, Statement of Cash Flows (Topic 230): Restricted Cash (“ASU 2016-18”), which enhances and clarifies the guidance on the classification and presentation of restricted cash in the statement of cash flows. The Company will adopt ASU 2016-18 in its first quarter of 2019 utilizing the retrospective adoption method. Currently, the Company's restricted cash balance is not significant. Income Taxes In October 2016, the FASB issued ASU No. 2016-16, Income Taxes (Topic 740): Intra-Entity Transfers of Assets Other Than Inventory (“ASU 2016-16”), which requires the recognition of the income tax consequences of an intra-entity transfer of an asset, other than inventory, when the transfer occurs. The Company will adopt ASU 2016-16 in its first quarter of 2019 utilizing the modified retrospective adoption method. Currently, the Company anticipates recording up to $9 billion of net deferred tax assets on its Consolidated Balance Sheets. However, the ultimate impact of adopting ASU 2016-16 will depend on the balance of intellectual property transferred between its subsidiaries as of the adoption date. The Company will recognize incremental deferred income tax expense thereafter as these deferred tax assets are utilized. Stock Compensation In March 2016, the FASB issued ASU No. 2016-09, Compensation – Stock Compensation (Topic 718): Improvements to Employee Share-Based Payment Accounting (“ASU 2016-09”), which modifies certain aspects of the accounting for share-based payment transactions, including income taxes, classification of awards, and classification in the statement of cash flows. The Company will adopt ASU 2016-09 in its first quarter of 2018. Currently, excess tax benefits or deficiencies from the Company's equity awards are recorded as additional paid-in capital in its Consolidated Balance Sheets. Upon adoption, the Company will record any excess tax benefits or deficiencies from its equity awards in its Consolidated Statements of Operations in the reporting periods in which vesting occurs. As a result, subsequent to adoption the Company's income tax expense and associated effective tax rate will be impacted by fluctuations in stock price between the grant dates and vesting dates of equity awards. Leases In February 2016, the FASB issued ASU No. 2016-02, Leases (Topic 842) (“ASU 2016-02”), which modifies lease accounting for lessees to increase transparency and comparability by recording lease assets and liabilities for operating leases and disclosing key information about leasing arrangements. ASU 2016-02 will be effective for the Company beginning in its first quarter of 2020, and early adoption is permitted. The Company will use a modified retrospective adoption approach. While the Company is currently evaluating the timing and impact of adopting ASU 2016-02, currently the Company anticipates recording lease assets and liabilities in excess of $7.5 billion on its Consolidated Balance Sheets, with no material impact to its Consolidated Statements of Operations. However, the ultimate impact of adopting ASU 2016-02 will depend on the Company's lease portfolio as of the adoption date. Financial Instruments In January 2016, the FASB issued ASU No. 2016-01, Financial Instruments – Overall (Subtopic 825-10): Recognition and Measurement of Financial Assets and Financial Liabilities (“ASU 2016-01”), which updates certain aspects of recognition, measurement, presentation and disclosure of financial instruments. The Company will adopt ASU 2016-01 in its first quarter of 2019 utilizing the modified retrospective adoption method. Based on the composition of the Company's investment portfolio, the adoption of ASU 2016-01 is not expected to have a material impact on its consolidated financial statements. 28 In June 2016, the FASB issued ASU No. 2016-13, Financial Instruments – Credit Losses (Topic 326): Measurement of Credit Losses on Financial Instruments (“ASU 2016-13”), which modifies the measurement of expected credit losses of certain financial instruments. The Company will adopt ASU 2016-13 in its first quarter of 2021 utilizing the modified retrospective adoption method. Based on the composition of the Company's investment portfolio, current market conditions, and historical credit loss activity, the adoption of ASU 2016-13 is not expected to have a material impact on its consolidated financial statements. Revenue Recognition In May 2014, the FASB issued ASU No. 2014-09, Revenue from Contracts with Customers (Topic 606) (“ASU 2014-09”), which amends the existing accounting standards for revenue recognition. ASU 2014-09 is based on principles that govern the recognition of revenue at an amount an entity expects to be entitled when products are transferred to customers. Subsequently, the FASB has issued the following standards related to ASU 2014-09: ASU No. 2016-08, Revenue from Contracts with Customers (Topic 606): Principal versus Agent Considerations (“ASU 2016-08”); ASU No. 2016-10, Revenue from Contracts with Customers (Topic 606): Identifying Performance Obligations and Licensing (“ASU 2016-10”); ASU No. 2016-12, Revenue from Contracts with Customers (Topic 606): Narrow-Scope Improvements and Practical Expedients (“ASU 2016-12”); and ASU No. 2016-20, Technical Corrections and Improvements to Topic 606, Revenue from Contracts with Customers (“ASU 2016-20”). The Company must adopt ASU 2016-08, ASU 2016-10, ASU 2016-12 and ASU 2016-20 with ASU 2014-09 (collectively, the “new revenue standards”). The new revenue standards may be applied retrospectively to each prior period presented or retrospectively with the cumulative effect recognized as of the date of adoption. The Company currently expects to adopt the new revenue standards in its first quarter of 2018 utilizing the full retrospective adoption method. The new revenue standards are not expected to have a material impact on the amount and timing of revenue recognized in the Company's consolidated financial statements. Liquidity and Capital Resources The following tables present selected financial information and statistics as of December 31, 2016 and September 24, 2016 and for the first three months of 2017 and 2016 (in millions): December 31, 2016 September 24, 2016 Cash, cash equivalents and marketable securities $ 246,090 $ 237,585 Property, plant and equipment, net $ 26,510 $ 27,010 Commercial paper $ 10,493 $ 8,105 Total term debt $ 77,056 $ 78,927 Working capital $ 19,202 $ 27,863 Three Months Ended December 31, 2016 December 26, 2015 Cash generated by operating activities $ 27,056 $ 27,463 Cash used in investing activities $ (19,122 ) $ (20,450 ) Cash used in financing activities $ (12,047 ) $ (11,444 ) The Company believes its existing balances of cash, cash equivalents and marketable securities will be sufficient to satisfy its working capital needs, capital asset purchases, outstanding commitments and other liquidity requirements associated with its existing operations over the next 12 months. The Company currently anticipates the cash used for future dividends, the share repurchase program and debt repayments will come from its current domestic cash, cash generated from on-going U.S. operating activities and from borrowings. As of December 31, 2016 and September 24, 2016, the Company’s cash, cash equivalents and marketable securities held by foreign subsidiaries were $230.2 billion and $216.0 billion, respectively, and are generally based in U.S. dollar-denominated holdings. Amounts held by foreign subsidiaries are generally subject to U.S. income taxation on repatriation to the U.S. In connection with the State Aid Decision, the European Commission announced a recovery amount of up to €13 billion, plus interest. The actual amount of additional taxes subject to recovery is to be calculated by Ireland in accordance with the European Commission's guidance. Once the recovery amount is computed by Ireland, the Company anticipates funding it, including interest, out of foreign cash into escrow, where it will remain pending conclusion of all appeals. The Company’s marketable securities investment portfolio is invested primarily in highly-rated securities, and its investment policy generally limits the amount of credit exposure to any one issuer. The policy requires investments generally to be investment grade with the objective of minimizing the potential risk of principal loss. 29 During the three months ended December 31, 2016, cash generated from operating activities of $27.1 billion was a result of $17.9 billion of net income, non-cash adjustments to net income of $5.4 billion and an increase in the net change in operating assets and liabilities of $3.7 billion. Cash used in investing activities of $19.1 billion during the three months ended December 31, 2016 consisted primarily of cash used for purchases of marketable securities, net of sales and maturities, of $15.6 billion and cash used to acquire property, plant and equipment of $3.3 billion. Cash used in financing activities of $12.0 billion during the three months ended December 31, 2016 consisted primarily of cash used to repurchase common stock of $10.9 billion and cash used to pay dividends and dividend equivalents of $3.1 billion, partially offset by a net increase in commercial paper of $2.4 billion. During the three months ended December 26, 2015, cash generated from operating activities of $27.5 billion was a result of $18.4 billion of net income, non-cash adjustments to net income of $5.7 billion and an increase in the net change in operating assets and liabilities of $3.4 billion. Cash used in investing activities of $20.5 billion during the three months ended December 26, 2015 consisted primarily of cash used for purchases of marketable securities, net of sales and maturities, of $16.1 billion and cash used to acquire property, plant and equipment of $3.6 billion. Cash used in financing activities of $11.4 billion during the three months ended December 26, 2015 consisted primarily of cash used to repurchase common stock of $6.9 billion, and cash used to pay dividends and dividend equivalents of $3.0 billion. Capital Assets The Company’s capital expenditures were $2.1 billion during the first quarter of 2017. The Company anticipates utilizing approximately $16.0 billion for capital expenditures during 2017, which includ</t>
-  </si>
-  <si>
     <t>Item 7. Management’s Discussion and Analysis of Financial Condition and Results of Operations This section and other parts of this Annual Report on Form 10-K (“Form 10-K”) contain forward-looking statements, within the meaning of the Private Securities Litigation Reform Act of 1995, that involve risks and uncertainties. Forward-looking statements provide current expectations of future events based on certain assumptions and include any statement that does not directly relate to any historical or current fact. Forward-looking statements can also be identified by words such as “future,” “anticipates,” “believes,” “estimates,” “expects,” “intends,” “plans,” “predicts,” “will,” “would,” “could,” “can,” “may,” and similar terms. Forward-looking statements are not guarantees of future performance and the Company’s actual results may differ significantly from the results discussed in the forward-looking statements. Factors that might cause such differences include, but are not limited to, those discussed in Part I, Item 1A of this Form 10-K under the heading “Risk Factors,” which are incorporated herein by reference. The following discussion should be read in conjunction with the consolidated financial statements and notes thereto included in Part II, Item 8 of this Form 10-K. All information presented herein is based on the Company’s fiscal calendar. Unless otherwise stated, references to particular years, quarters, months or periods refer to the Company’s fiscal years ended in September and the associated quarters, months and periods of those fiscal years. Each of the terms the “Company” and “Apple” as used herein refers collectively to Apple Inc. and its wholly-owned subsidiaries, unless otherwise stated. The Company assumes no obligation to revise or update any forward-looking statements for any reason, except as required by law. Overview and Highlights The Company designs, manufactures and markets mobile communication and media devices, personal computers and portable digital music players, and sells a variety of related software, services, accessories, networking solutions and third-party digital content and applications. The Company’s products and services include iPhone®, iPad®, Mac®, iPod®, Apple Watch®, Apple TV®, a portfolio of consumer and professional software applications, iOS, macOS™, watchOS® and tvOS™ operating systems, iCloud®, Apple Pay® and a variety of accessory, service and support offerings. The Company sells and delivers digital content and applications through the iTunes Store®, App Store®, Mac App Store, TV App Store, iBooks Store™ and Apple Music® (collectively “Internet Services”). The Company sells its products worldwide through its retail stores, online stores and direct sales force, as well as through third-party cellular network carriers, wholesalers, retailers and value-added resellers. In addition, the Company sells a variety of third-party Apple compatible products, including application software and various accessories through its retail and online stores. The Company sells to consumers, small and mid-sized businesses and education, enterprise and government customers. Fiscal 2016 Highlights Net sales declined 8% or $18.1 billion during 2016 compared to 2015, primarily driven by a year-over-year decrease in iPhone net sales and the effect of weakness in most foreign currencies relative to the U.S. dollar, partially offset by an increase in Services. In April 2016, the Company announced a significant increase to its capital return program by raising the expected total size of the program from $200 billion to $250 billion through March 2018. This included increasing its share repurchase authorization from $140 billion to $175 billion and raising its quarterly dividend from $0.52 to $0.57 per share beginning in May 2016. During 2016, the Company spent $29.0 billion to repurchase shares of its common stock and paid dividends and dividend equivalents of $12.2 billion. Additionally, the Company issued $23.9 billion of U.S. dollar-denominated term debt and A$1.4 billion of Australian dollar-denominated term debt during 2016. Fiscal 2015 Highlights Net sales rose 28% or $50.9 billion during 2015 compared to 2014, driven by a year-over-year increase in iPhone net sales. iPhone net sales and unit sales in 2015 increased in all of the Company’s reportable operating segments. The Company also experienced year-over-year net sales increases in Mac, Services and Other Products. Apple Watch, which launched during the third quarter of 2015, accounted for more than 100% of the year-over-year growth in net sales of Other Products. Net sales growth during 2015 was partially offset by the effect of weakness in most foreign currencies relative to the U.S. dollar and lower iPad net sales. Total net sales increased in each of the Company’s reportable operating segments, with particularly strong growth in Greater China where year-over-year net sales increased 84%. In April 2015, the Company announced a significant increase to its capital return program by raising the expected total size of the program to $200 billion through March 2017. This included increasing its share repurchase authorization to $140 billion and raising its quarterly dividend to $0.52 per share beginning in May 2015. During 2015, the Company spent $36.0 billion to repurchase shares of its common stock and paid dividends and dividend equivalents of $11.6 billion. Additionally, the Company issued $14.5 billion of U.S. dollar-denominated, €4.8 billion of euro-denominated, SFr1.3 billion of Swiss franc-denominated, £1.3 billion of British pound-denominated, A$2.3 billion of Australian dollar-denominated and ¥250.0 billion of Japanese yen-denominated term debt during 2015. Apple Inc. | 2016 Form 10-K | 22 Sales Data The following table shows net sales by operating segment and net sales and unit sales by product during 2016, 2015 and 2014 (dollars in millions and units in thousands): 2016 Change 2015 Change 2014 Net Sales by Operating Segment: Americas $ 86,613 (8 )% $ 93,864 17 % $ 80,095 Europe 49,952 (1 )% 50,337 14 % 44,285 Greater China 48,492 (17 )% 58,715 84 % 31,853 Japan 16,928 8 % 15,706 3 % 15,314 Rest of Asia Pacific 13,654 (10 )% 15,093 34 % 11,248 Total net sales $ 215,639 (8 )% $ 233,715 28 % $ 182,795 Net Sales by Product: iPhone (1) $ 136,700 (12 )% $ 155,041 52 % $ 101,991 iPad (1) 20,628 (11 )% 23,227 (23 )% 30,283 Mac (1) 22,831 (10 )% 25,471 6 % 24,079 Services (2) 24,348 22 % 19,909 10 % 18,063 Other Products (1)(3) 11,132 11 % 10,067 20 % 8,379 Total net sales $ 215,639 (8 )% $ 233,715 28 % $ 182,795 Unit Sales by Product: iPhone 211,884 (8 )% 231,218 37 % 169,219 iPad 45,590 (17 )% 54,856 (19 )% 67,977 Mac 18,484 (10 )% 20,587 9 % 18,906 (1) Includes deferrals and amortization of related software upgrade rights and non-software services. (2) Includes revenue from Internet Services, AppleCare®, Apple Pay, licensing and other services. (3) Includes sales of Apple TV, Apple Watch, Beats® products, iPod and Apple-branded and third-party accessories. Apple Inc. | 2016 Form 10-K | 23 Product Performance iPhone The following table presents iPhone net sales and unit sales information for 2016, 2015 and 2014 (dollars in millions and units in thousands): 2016 Change 2015 Change 2014 Net sales $ 136,700 (12 )% $ 155,041 52 % $ 101,991 Percentage of total net sales 63 % 66 % 56 % Unit sales 211,884 (8 )% 231,218 37 % 169,219 iPhone net sales and unit sales decreased during 2016 compared to 2015. The Company believes the sales decline is due primarily to a lower rate of iPhone upgrades during 2016 compared to 2015 and challenging macroeconomic conditions in a number of major markets in 2016. Average selling prices (“ASPs”) for iPhone were lower year-over-year during 2016 due primarily to a different mix of iPhones, including the iPhone SE introduced in 2016, and the effect of weakness in most foreign currencies relative to the U.S. dollar. The year-over-year growth in iPhone net sales and unit sales during 2015 primarily resulted from strong demand for iPhone 6 and 6 Plus during 2015. Overall ASPs for iPhone increased during 2015 compared to 2014, due primarily to the introduction of iPhone 6 and 6 Plus in September 2014, partially offset by the effect of weakness in most foreign currencies relative to the U.S. dollar. iPad The following table presents iPad net sales and unit sales information for 2016, 2015 and 2014 (dollars in millions and units in thousands): 2016 Change 2015 Change 2014 Net sales $ 20,628 (11 )% $ 23,227 (23 )% $ 30,283 Percentage of total net sales 10 % 10 % 17 % Unit sales 45,590 (17 )% 54,856 (19 )% 67,977 iPad net sales decreased during 2016 compared to 2015 primarily due to lower unit sales and the effect of weakness in most foreign currencies relative to the U.S. dollar, partially offset by higher ASPs due to a shift in mix to higher-priced iPads. The Company believes the decline in iPad sales is due in part to a longer repurchase cycle for iPads and some level of cannibalization from the Company's other products. Net sales and unit sales for iPad declined during 2015 compared to 2014. The Company believes the decline in iPad sales is due in part to a longer repurchase cycle for iPads and some level of cannibalization from the Company's other products. iPad ASPs declined during 2015 compared to 2014, primarily as a result of the effect of weakness in most foreign currencies relative to the U.S. dollar and a shift in mix to lower-priced iPads. Mac The following table presents Mac net sales and unit sales information for 2016, 2015 and 2014 (dollars in millions and units in thousands): 2016 Change 2015 Change 2014 Net sales $ 22,831 (10 )% $ 25,471 6 % $ 24,079 Percentage of total net sales 11 % 11 % 13 % Unit sales 18,484 (10 )% 20,587 9 % 18,906 Mac net sales and unit sales decreased during 2016 compared to 2015. The year-over-year decline in Mac unit sales during 2016 was at rates similar to the overall market. The effect of weakness in most foreign currencies relative to the U.S. dollar also negatively impacted Mac net sales. The year-over-year growth in Mac net sales and unit sales during 2015 was driven by strong demand for Mac portables. Mac ASPs declined during 2015 compared to 2014 largely due to the effect of weakness in most foreign currencies relative to the U.S. dollar. Apple Inc. | 2016 Form 10-K | 24 Services The following table presents net sales information of Services for 2016, 2015 and 2014 (dollars in millions): 2016 Change 2015 Change 2014 Net sales $ 24,348 22 % $ 19,909 10 % $ 18,063 Percentage of total net sales 11 % 9 % 10 % The year-over-year increase in net sales of Services in 2016 was due primarily to growth from the App Store, licensing and AppleCare sales, partially offset by the effect of weakness in most foreign currencies relative to the U.S. dollar. During the first quarter of 2016, the Company received $548 million from Samsung Electronics Co., Ltd. related to its patent infringement lawsuit, which was recorded as licensing net sales within Services. The increase in net sales of Services during 2015 compared to 2014 was primarily due to growth from the App Store and licensing. Segment Operating Performance The Company manages its business primarily on a geographic basis. The Company’s reportable operating segments consist of the Americas, Europe, Greater China, Japan and Rest of Asia Pacific. The Americas segment includes both North and South America. The Europe segment includes European countries, as well as India, the Middle East and Africa. The Greater China segment includes China, Hong Kong and Taiwan. The Rest of Asia Pacific segment includes Australia and those Asian countries not included in the Company’s other reportable operating segments. Although the reportable operating segments provide similar hardware and software products and similar services, each one is managed separately to better align with the location of the Company’s customers and distribution partners and the unique market dynamics of each geographic region. Further information regarding the Company’s reportable operating segments can be found in Part II, Item 8 of this Form 10-K in the Notes to Consolidated Financial Statements in Note 11, “Segment Information and Geographic Data.” Americas The following table presents Americas net sales information for 2016, 2015 and 2014 (dollars in millions): 2016 Change 2015 Change 2014 Net sales $ 86,613 (8 )% $ 93,864 17 % $ 80,095 Percentage of total net sales 40 % 40 % 44 % Americas net sales decreased during 2016 compared to 2015 due primarily to lower net sales and unit sales of iPhone. The year-over-year growth in Americas net sales during 2015 was driven primarily by growth in net sales and unit sales of iPhone, partially offset by a decline in net sales and unit sales of iPad. Europe The following table presents Europe net sales information for 2016, 2015 and 2014 (dollars in millions): 2016 Change 2015 Change 2014 Net sales $ 49,952 (1 )% $ 50,337 14 % $ 44,285 Percentage of total net sales 23 % 22 % 24 % Europe net sales decreased during 2016 compared to 2015 driven primarily by the effect of weakness in foreign currencies relative to the U.S. dollar and a decrease in unit sales of Mac, largely offset by an increase in iPhone unit sales and Services. The year-over-year increase in Europe net sales during 2015 was driven primarily by growth in net sales and unit sales of iPhone, partially offset by the effect of weakness in foreign currencies relative to the U.S. dollar and a decline in net sales and unit sales of iPad. Apple Inc. | 2016 Form 10-K | 25 Greater China The following table presents Greater China net sales information for 2016, 2015 and 2014 (dollars in millions): 2016 Change 2015 Change 2014 Net sales $ 48,492 (17 )% $ 58,715 84 % $ 31,853 Percentage of total net sales 22 % 25 % 17 % Greater China net sales decreased during 2016 compared to 2015 due primarily to lower net sales and unit sales of iPhone and the effect of weakness in foreign currencies relative to the U.S. dollar. Greater China experienced strong year-over-year increases in net sales during 2015 driven primarily by iPhone sales. Japan The following table presents Japan net sales information for 2016, 2015 and 2014 (dollars in millions): 2016 Change 2015 Change 2014 Net sales $ 16,928 8 % $ 15,706 3 % $ 15,314 Percentage of total net sales 8 % 7 % 8 % Japan net sales increased during 2016 compared to 2015 due primarily to higher net sales of Services and the strength in the Japanese yen relative to the U.S. dollar. The year-over-year increase in Japan net sales during 2015 was driven primarily by growth in Services largely associated with strong App Store sales, partially offset by the effect of weakness in the Japanese yen relative to the U.S. dollar. Rest of Asia Pacific The following table presents Rest of Asia Pacific net sales information for 2016, 2015 and 2014 (dollars in millions): 2016 Change 2015 Change 2014 Net sales $ 13,654 (10 )% $ 15,093 34 % $ 11,248 Percentage of total net sales 6 % 6 % 6 % Rest of Asia Pacific net sales decreased during 2016 compared to 2015 due primarily to lower net sales and unit sales of iPhone and the effect of weakness in foreign currencies relative to the U.S. dollar. The year-over-year increase in Rest of Asia Pacific net sales during 2015 primarily reflects strong growth in net sales and unit sales of iPhone, partially offset by the effect of weakness in foreign currencies relative to the U.S. dollar and a decline in net sales and unit sales of iPad. Gross Margin Gross margin for 2016, 2015 and 2014 is as follows (dollars in millions): 2016 2015 2014 Net sales $ 215,639 $ 233,715 $ 182,795 Cost of sales 131,376 140,089 112,258 Gross margin $ 84,263 $ 93,626 $ 70,537 Gross margin percentage 39.1 % 40.1 % 38.6 % Gross margin decreased in 2016 compared to 2015 due primarily to the effect of weakness in most foreign currencies relative to the U.S. dollar and, to a lesser extent, unfavorable leverage on fixed costs from lower net sales, partially offset by a favorable shift in mix to Services. The year-over-year increase in the gross margin percentage in 2015 was driven primarily by a favorable shift in mix to products with higher margins and, to a lesser extent, by improved leverage on fixed costs from higher net sales. These positive factors were partially offset primarily by higher product cost structures and, to a lesser extent, by the effect of weakness in most foreign currencies relative to the U.S. dollar. Apple Inc. | 2016 Form 10-K | 26 The Company anticipates gross margin during the first quarter of 2017 to be between 38% and 38.5%. The foregoing statement regarding the Company’s expected gross margin percentage in the first quarter of 2017 is forward-looking and could differ from actual results. The Company’s future gross margins can be impacted by multiple factors including, but not limited to, those set forth in Part I, Item 1A of this Form 10-K under the heading “Risk Factors” and those described in this paragraph. In general, the Company believes gross margins will remain under downward pressure due to a variety of factors, including continued industry wide global product pricing pressures, increased competition, compressed product life cycles, product transitions, potential increases in the cost of components, and potential strengthening of the U.S. dollar, as well as potential increases in the costs of outside manufacturing services and a potential shift in the Company’s sales mix towards products with lower gross margins. In response to competitive pressures, the Company expects it will continue to take product pricing actions, which would adversely affect gross margins. Gross margins could also be affected by the Company’s ability to manage product quality and warranty costs effectively and to stimulate demand for certain of its products. Due to the Company’s significant international operations, its financial condition and operating results, including gross margins, could be significantly affected by fluctuations in exchange rates. Operating Expenses Operating expenses for 2016, 2015 and 2014 are as follows (dollars in millions): 2016 Change 2015 Change 2014 Research and development $ 10,045 25 % $ 8,067 34 % $ 6,041 Percentage of total net sales 5 % 3 % 3 % Selling, general and administrative $ 14,194 (1 )% $ 14,329 19 % $ 11,993 Percentage of total net sales 7 % 6 % 7 % Total operating expenses $ 24,239 8 % $ 22,396 24 % $ 18,034 Percentage of total net sales 11 % 10 % 10 % Research and Development The year-over-year growth in R&amp;D expense in 2016 and 2015 was driven primarily by an increase in headcount and related expenses, and material costs to support expanded R&amp;D activities. The Company continues to believe that focused investments in R&amp;D are critical to its future growth and competitive position in the marketplace, and to the development of new and updated products that are central to the Company’s core business strategy. Selling, General and Administrative The decrease in selling, general and administrative expense in 2016 compared to 2015 was due primarily to lower discretionary expenditures and advertising costs, partially offset by an increase in headcount and related expenses. The year-over-year growth in selling, general and administrative expense in 2015 was primarily due to increased headcount and related expenses, and higher spending on marketing and advertising. Other Income/(Expense), Net Other income/(expense), net for 2016, 2015 and 2014 are as follows (dollars in millions): 2016 Change 2015 Change 2014 Interest and dividend income $ 3,999 $ 2,921 $ 1,795 Interest expense (1,456 ) (733 ) (384 ) Other expense, net (1,195 ) (903 ) (431 ) Total other income/(expense), net $ 1,348 5 % $ 1,285 31 % $ 980 The year-over-year increase in other income/(expense), net during 2016 and 2015 was due primarily to higher interest income, partially offset by higher interest expense on debt and higher expenses associated with foreign exchange activity. The weighted-average interest rate earned by the Company on its cash, cash equivalents and marketable securities was 1.73%, 1.49% and 1.11% in 2016, 2015 and 2014, respectively. Apple Inc. | 2016 Form 10-K | 27 Provision for Income Taxes Provision for income taxes and effective tax rates for 2016, 2015 and 2014 are as follows (dollars in millions): 2016 2015 2014 Provision for income taxes 15,685 $ 19,121 $ 13,973 Effective tax rate 25.6 % 26.4 % 26.1 % The Company’s effective tax rates for 2016, 2015 and 2014 differ from the statutory federal income tax rate of 35% due primarily to certain undistributed foreign earnings, a substantial portion of which was generated by subsidiaries organized in Ireland, for which no U.S. taxes are provided when such earnings are intended to be indefinitely reinvested outside the U.S. The lower effective tax rate in 2016 compared to 2015 was due primarily to greater R&amp;D tax credits. The higher effective tax rate during 2015 compared to 2014 was due primarily to higher foreign taxes. As of September 24, 2016, the Company had deferred tax assets arising from deductible temporary differences, tax losses and tax credits of $4.1 billion and deferred tax liabilities of $26.0 billion. Management believes it is more likely than not that forecasted income, including income that may be generated as a result of certain tax planning strategies, together with future reversals of existing taxable temporary differences, will be sufficient to fully recover the deferred tax assets. The Company will continue to evaluate the realizability of deferred tax assets quarterly by assessing the need for and the amount of a valuation allowance. During the fourth quarter of 2016, the Company reached a partial settlement with the IRS on its examination of the years 2010 through 2012. In connection with this settlement, the Company recognized a tax benefit in the fourth quarter of 2016 that was not significant to its consolidated financial statements. All years prior to 2013 are closed, except for the years 2010 through 2012 relating to R&amp;D tax credits. In addition, the Company is subject to audits by state, local and foreign tax authorities. In major states and major foreign jurisdictions, the years subsequent to 2003 generally remain open and could be subject to examination by the taxing authorities. Management believes that adequate provisions have been made for any adjustments that may result from tax examinations. However, the outcome of tax audits cannot be predicted with certainty. If any issues addressed in the Company’s tax audits are resolved in a manner not consistent with management’s expectations, the Company could be required to adjust its provision for income taxes in the period such resolution occurs. On August 30, 2016, the European Commission announced its decision that Ireland granted state aid to the Company by providing tax opinions in 1991 and 2007 concerning the tax allocation of profits of the Irish branches of two subsidiaries of the Company (the "State Aid Decision"). The State Aid Decision orders Ireland to calculate and recover additional taxes from the Company for the period June 2003 through September 2014. Irish legislative changes, effective as of the beginning of 2015, eliminated the application of the tax opinions from that date forward. The Company believes the State Aid Decision to be without merit and intends to appeal to the General Court of the Court of Justice of the European Union. Ireland has also announced its intention to appeal the State Aid Decision. While the European Commission announced a recovery amount of up to €13 billion, plus interest, the actual amount of additional taxes subject to recovery is to be calculated by Ireland in accordance with the European Commission's guidance. Once the recovery amount is computed by Ireland, the Company anticipates funding it, including interest, out of foreign cash into escrow, pending conclusion of all appeals. The Company believes that any incremental Irish corporate income taxes potentially due would be creditable against U.S. taxes. Recent Accounting Pronouncements Income Taxes In October 2016, the Financial Accounting Standards Board (“FASB”) issued Accounting Standards Update (“ASU”) 2016-16, Income Taxes (Topic 740): Intra-Entity Transfer of Assets Other than Inventory ("ASU 2016-16"), which requires the recognition of the income tax consequences of an intra-entity transfer of an asset, other than inventory, when the transfer occurs. ASU 2016-06 will be effective for the Company in its first quarter of 2019. The Company is currently evaluating the impact of adopting ASU 2016-16 on its consolidated financial statements. Stock Compensation In March 2016, the FASB issued ASU No. 2016-09, Compensation – Stock Compensation (Topic 718): Improvements to Employee Share-Based Payment Accounting (“ASU 2016-09”), which simplified certain aspects of the accounting for share-based payment transactions, including income taxes, classification of awards and classification on the statement of cash flows. ASU 2016-09 will be effective for the Company beginning in its first quarter of 2018. The Company is currently evaluating the impact of adopting ASU 2016-09 on its consolidated financial statements. Apple Inc. | 2016 Form 10-K | 28 Leases In February 2016, the FASB issued ASU No. 2016-02, Leases (Topic 842) (“ASU 2016-02”), which modified lease accounting for both lessees and lessors to increase transparency and comparability by recognizing lease assets and lease liabilities by lessees for those leases classified as operating leases under previous accounting standards and disclosing key information about leasing arrangements. ASU 2016-02 will be effective for the Company beginning in its first quarter of 2020, and early adoption is permitted. The Company is currently evaluating the timing of its adoption and the impact of adopting ASU 2016-02 on its consolidated financial statements. Financial Instruments In January 2016, the FASB issued ASU No. 2016-01, Financial Instruments – Overall (Subtopic 825-10): Recognition and Measurement of Financial Assets and Financial Liabilities (“ASU 2016-01”), which updates certain aspects of recognition, measurement, presentation and disclosure of financial instruments. ASU 2016-01 will be effective for the Company beginning in its first quarter of 2019. The Company does not believe the adoption of ASU 2016-01 will have a material impact on its consolidated financial statements. In June 2016, the FASB issued ASU No. 2016-13, Financial Instruments – Credit Losses (Topic 326): Measurement of Credit Losses on Financial Instruments (“ASU 2016-13”), which modifies the measurement of expected credit losses of certain financial instruments. ASU 2016-13 will be effective for the Company beginning in its first quarter of 2021 and early adoption is permitted. The Company does not believe the adoption of ASU 2016-13 will have a material impact on its consolidated financial statements. Revenue Recognition In May 2014, the FASB issued ASU No. 2014-09, Revenue from Contracts with Customers (Topic 606) (“ASU 2014-09”), which amends the existing accounting standards for revenue recognition. ASU 2014-09 is based on principles that govern the recognition of revenue at an amount an entity expects to be entitled when products are transferred to customers. ASU 2014-09 will be effective for the Company beginning in its first quarter of 2019, and early adoption is permitted. Subsequently, the FASB has issued the following standards related to ASU 2014-09: ASU No. 2016-08, Revenue from Contracts with Customers (Topic 606): Principal versus Agent Considerations (“ASU 2016-08”); ASU No. 2016-10, Revenue from Contracts with Customers (Topic 606): Identifying Performance Obligations and Licensing (“ASU 2016-10”); and ASU No. 2016-12, Revenue from Contracts with Customers (Topic 606): Narrow-Scope Improvements and Practical Expedients (“ASU 2016-12”). The Company must adopt ASU 2016-08, ASU 2016-10 and ASU 2016-12 with ASU 2014-09 (collectively, the “new revenue standards”). The new revenue standards may be applied retrospectively to each prior period presented or retrospectively with the cumulative effect recognized as of the date of adoption. The Company currently expects to adopt the new revenue standards in its first quarter of 2018 utilizing the full retrospective transition method. The Company does not expect adoption of the new revenue standards to have a material impact on its consolidated financial statements. Liquidity and Capital Resources The following table presents selected financial information and statistics as of and for the years ended September 24, 2016, September 26, 2015 and September 27, 2014 (in millions): 2016 2015 2014 Cash, cash equivalents and marketable securities $ 237,585 $ 205,666 $ 155,239 Property, plant and equipment, net $ 27,010 $ 22,471 $ 20,624 Commercial paper $ 8,105 $ 8,499 $ 6,308 Total term debt $ 78,927 $ 55,829 $ 28,987 Working capital $ 27,863 $ 8,768 $ 5,083 Cash generated by operating activities $ 65,824 $ 81,266 $ 59,713 Cash used in investing activities $ (45,977 ) $ (56,274 ) $ (22,579 ) Cash used in financing activities $ (20,483 ) $ (17,716 ) $ (37,549 ) The Company believes its existing balances of cash, cash equivalents and marketable securities will be sufficient to satisfy its working capital needs, capital asset purchases, outstanding commitments and other liquidity requirements associated with its existing operations over the next 12 months. The Company currently anticipates the cash used for future dividends, the share repurchase program and debt repayments will come from its current domestic cash, cash generated from on-going U.S. operating activities and from borrowings. Apple Inc. | 2016 Form 10-K | 29 As of September 24, 2016 and September 26, 2015, the Company’s cash, cash equivalents and marketable securities held by foreign subsidiaries were $216.0 billion and $186.9 billion, respectively, and are generally based in U.S. dollar-denominated holdings. Amounts held by foreign subsidiaries are generally subject to U.S. income taxation on repatriation to the U.S. In connection with the State Aid Decision, the European Commission announced a recovery amount of up to €13 billion, plus interest. The actual amount of additional taxes subject to recovery is to be calculated by Ireland in accordance with the European Commission's guidance. Once the recovery amount is computed by Ireland, the Company anticipates funding it, including interest, out of foreign cash into escrow, pending conclusion of all appeals. The Company’s marketable securities investment portfolio is invested primarily in highly-rated securities and its investment policy generally limits the amount of credit exposure to any one issuer. The policy requires investments generally to be investment grade with the objective of minimizing the potential risk of principal loss. During 2016, cash generated from operating activities of $65.8 billion was a result of $45.7 billion of net income, non-cash adjustments to net income of $19.7 billion and an increase in the net change in operating assets and liabilities of $484 million. Cash used in investing activities of $46.0 billion during 2016 consisted primarily of cash used for purchases of marketable securities, net of sales and maturities, of $30.6 billion and cash used to acquire property, plant and equipment of $12.7 billion. Cash used in financing activities of $20.5 billion during 2016 consisted primarily of cash used to repurchase common stock of $29.7 billion, cash used to pay dividends and dividend equivalents of $12.2 billion and cash used to repay term debt of $2.5 billion, partially offset by net proceeds from the issuance of term debt of $25.0 billion. During 2015, cash generated from operating activities of $81.3 billion was a result of $53.4 billion of net income, non-cash adjustments to net income of $16.2 billion and an increase in the net change in operating assets and liabilities of $11.6 billion. Cash used in investing activities of $56.3 billion during 2015 consisted primarily of cash used for purchases of marketable securities, net of sales and maturities, of $44.4 billion and cash used to acquire property, plant and equipment of $11.2 billion. Cash used in financing activities of $17.7 billion during 2015 consisted primarily of cash used to repurchase common stock of $35.3 billion and cash used to pay dividends and dividend equivalents of $11.6 billion, partially offset by net proceeds from the issuance of term deb</t>
+  </si>
+  <si>
+    <t>Item 2. Management’s Discussion and Analysis of Financial Condition and Results of Operations This section and other parts of this Quarterly Report on Form 10‑Q contain forward-looking statements, within the meaning of the Private Securities Litigation Reform Act of 1995, that involve risks and uncertainties. Forward-looking statements provide current expectations of future events based on certain assumptions and include any statement that does not directly relate to any historical or current fact. Forward-looking statements can also be identified by words such as “future,” “anticipates,” “believes,” “estimates,” “expects,” “intends,” “plans,” “predicts,” “will,” “would,” “could,” “can,” “may,” and similar terms. Forward-looking statements are not guarantees of future performance and the Company’s actual results may differ significantly from the results discussed in the forward-looking statements. Factors that might cause such differences include, but are not limited to, those discussed in Part II, Item 1A of this Form 10-Q under the heading “Risk Factors,” which are incorporated herein by reference. The following discussion should be read in conjunction with the Company’s Annual Report on Form 10-K for the year ended September 24, 2016 (the “2016 Form 10-K”) filed with the U.S. Securities and Exchange Commission (the “SEC”) and the condensed consolidated financial statements and notes thereto included elsewhere in this Form 10-Q. All information presented herein is based on the Company’s fiscal calendar. Unless otherwise stated, references to particular years, quarters, months or periods refer to the Company’s fiscal years ended in September and the associated quarters, months and periods of those fiscal years. Each of the terms the “Company” and “Apple” as used herein refers collectively to Apple Inc. and its wholly-owned subsidiaries, unless otherwise stated. The Company assumes no obligation to revise or update any forward-looking statements for any reason, except as required by law. Available Information The Company’s Annual Report on Form 10-K, Quarterly Reports on Form 10-Q, Current Reports on Form 8-K, and amendments to reports filed pursuant to Sections 13(a) and 15(d) of the Securities Exchange Act of 1934, as amended (the “Exchange Act”), are filed with the SEC. The Company is subject to the informational requirements of the Exchange Act and files or furnishes reports, proxy statements, and other information with the SEC. Such reports and other information filed by the Company with the SEC are available free of charge on the Company’s website at investor.apple.com/sec.cfm when such reports are available on the SEC’s website. The public may read and copy any materials filed by the Company with the SEC at the SEC’s Public Reference Room at 100 F Street, NE, Room 1580, Washington, DC 20549. The public may obtain information on the operation of the Public Reference Room by calling the SEC at 1-800-SEC-0330. The SEC maintains an internet site that contains reports, proxy and information statements and other information regarding issuers that file electronically with the SEC at www.sec.gov. The contents of websites are not incorporated into this filing. Further, the Company’s references to website URLs are intended to be inactive textual references only. Overview and Highlights The Company designs, manufactures and markets mobile communication and media devices, personal computers and portable digital music players, and sells a variety of related software, services, accessories, networking solutions and third-party digital content and applications. The Company’s products and services include iPhone®, iPad®, Mac®, iPod®, Apple Watch®, Apple TV®, a portfolio of consumer and professional software applications, iOS, macOS™, watchOS® and tvOS™ operating systems, iCloud®, Apple Pay® and a variety of accessory, service and support offerings. The Company sells and delivers digital content and applications through the iTunes Store®, App Store®, Mac App Store, TV App Store, iBooks Store™ and Apple Music® (collectively “Digital Content and Services”). The Company sells its products worldwide through its retail stores, online stores and direct sales force, as well as through third-party cellular network carriers, wholesalers, retailers and value-added resellers. In addition, the Company sells a variety of third-party Apple-compatible products, including application software and various accessories through its retail and online stores. The Company sells to consumers, small and mid-sized businesses and education, enterprise and government customers. Business Strategy The Company is committed to bringing the best user experience to its customers through its innovative hardware, software and services. The Company’s business strategy leverages its unique ability to design and develop its own operating systems, hardware, application software and services to provide its customers products and solutions with innovative design, superior ease-of-use and seamless integration. As part of its strategy, the Company continues to expand its platform for the discovery and delivery of digital content and applications through its Digital Content and Services, which allows customers to discover and download digital content, iOS, Mac, Apple Watch and Apple TV applications, and books through either a Mac or Windows personal computer or through iPhone, iPad and iPod touch® devices (“iOS devices”), Apple TV and Apple Watch. The Company also supports a community for the development of third-party software and hardware products and digital content that complement the Company’s offerings. The Company believes a high-quality buying experience with knowledgeable salespersons who can convey the value of the Company’s products and services greatly enhances its ability to attract and retain customers. Therefore, the Company’s strategy also includes building and expanding its own retail and online stores and its third-party distribution network to effectively reach more customers and provide them with a high-quality sales and post-sales support experience. The Company believes ongoing investment in research and development (“R&amp;D”), marketing and advertising is critical to the development and sale of innovative products and technologies. 22 Business Seasonality and Product Introductions The Company has historically experienced higher net sales in its first quarter compared to other quarters in its fiscal year due in part to seasonal holiday demand. Additionally, new product introductions can significantly impact net sales, product costs and operating expenses. Product introductions can also impact the Company’s net sales to its indirect distribution channels as these channels are filled with new product inventory following a product introduction, and often, channel inventory of a particular product declines as the next related major product launch approaches. Net sales can also be affected when consumers and distributors anticipate a product introduction. However, neither historical seasonal patterns nor historical patterns of product introductions should be considered reliable indicators of the Company’s future pattern of product introductions, future net sales or financial performance. Fiscal Period The Company’s fiscal year is the 52 or 53-week period that ends on the last Saturday of September. The Company’s fiscal year 2017 will include 53 weeks and will end on September 30, 2017. A 14th week has been included in the first quarter of 2017, as is done every five or six years, to realign the Company’s fiscal quarters with calendar quarters. First Quarter Fiscal 2017 Highlights Net sales grew 3% or $2.5 billion during the first quarter of 2017 compared to the first quarter of 2016, primarily driven by strong growth in iPhone and Services, partially offset by lower iPad sales. The positive impact of having an additional week in the first quarter of 2017 was primarily offset by lower year-over-year channel inventory growth, an earlier launch of iPhone 7 and 7 Plus as compared to the prior year and the effect of weakness in foreign currencies relative to the U.S. dollar. During the first quarter of 2017, the Company introduced a new MacBook Pro® with Touch Bar™, an interface that replaces the traditional row of function keys, and released AirPods™, which are new wireless headphones. Sales Data The following table shows net sales by operating segment and net sales and unit sales by product for the three months ended December 31, 2016 and December 26, 2015 (dollars in millions and units in thousands): Three Months Ended December 31, 2016 December 26, 2015 Change Net Sales by Operating Segment: Americas $ 31,968 $ 29,325 9 % Europe 18,521 17,932 3 % Greater China 16,233 18,373 (12 )% Japan 5,766 4,794 20 % Rest of Asia Pacific 5,863 5,448 8 % Total net sales $ 78,351 $ 75,872 3 % Net Sales by Product: iPhone (1) $ 54,378 $ 51,635 5 % iPad (1) 5,533 7,084 (22 )% Mac (1) 7,244 6,746 7 % Services (2) 7,172 6,056 18 % Other Products (1)(3) 4,024 4,351 (8 )% Total net sales $ 78,351 $ 75,872 3 % Unit Sales by Product: iPhone 78,290 74,779 5 % iPad 13,081 16,122 (19 )% Mac 5,374 5,312 1 % (1) Includes deferrals and amortization of related software upgrade rights and non-software services. (2) Includes revenue from Digital Content and Services, AppleCare®, Apple Pay, licensing and other services. (3) Includes sales of Apple TV, Apple Watch, Beats® products, iPod and Apple-branded and third-party accessories. 23 Product Performance iPhone The following table presents iPhone net sales and unit sales information for the first quarter of 2017 and 2016 (dollars in millions and units in thousands): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 54,378 $ 51,635 5 % Percentage of total net sales 69 % 68 % Unit sales 78,290 74,779 5 % iPhone net sales increased during the first quarter of 2017 compared to the same quarter in 2016, driven by strong growth in each of the geographic operating segments, with the exception of Greater China. iPad The following table presents iPad net sales and unit sales information for the first quarter of 2017 and 2016 (dollars in millions and units in thousands): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 5,533 $ 7,084 (22 )% Percentage of total net sales 7 % 9 % Unit sales 13,081 16,122 (19 )% iPad net sales decreased in the first quarter of 2017 compared to the same quarter in 2016 due to lower iPad unit sales and lower average selling prices for iPad, both due in part to the introduction of the 12.9-inch iPad Pro in the first quarter of 2016. Mac The following table presents Mac net sales and unit sales information for the first quarter of 2017 and 2016 (dollars in millions and units in thousands): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 7,244 $ 6,746 7 % Percentage of total net sales 9 % 9 % Unit sales 5,374 5,312 1 % Mac net sales increased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to a different mix of Macs, including the new MacBook Pro introduced in the first quarter of 2017. Services The following table presents Services net sales information for the first quarter of 2017 and 2016 (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 7,172 $ 6,056 18 % Percentage of total net sales 9 % 8 % The year-over-year increase in Services net sales in the first quarter of 2017 compared to the same quarter in 2016 was due primarily to growth from the App Store and AppleCare sales, partially offset by the $548 million received from Samsung Electronics Co., Ltd. in the first quarter of 2016 related to patent infringement matters. 24 Segment Operating Performance The Company manages its business primarily on a geographic basis. The Company’s reportable operating segments consist of the Americas, Europe, Greater China, Japan and Rest of Asia Pacific. The Americas segment includes both North and South America. The Europe segment includes European countries, as well as India, the Middle East and Africa. The Greater China segment includes China, Hong Kong and Taiwan. The Rest of Asia Pacific segment includes Australia and those Asian countries not included in the Company’s other reportable operating segments. Although the reportable operating segments provide similar hardware and software products and similar services, each one is managed separately to better align with the location of the Company’s customers and distribution partners and the unique market dynamics of each geographic region. Further information regarding the Company’s reportable operating segments can be found in Part I, Item 1 of this Form 10-Q in the Notes to Condensed Consolidated Financial Statements, in Note 11, “Segment Information and Geographic Data.” Americas The following table presents Americas net sales information for the first quarter of 2017 and 2016 (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 31,968 $ 29,325 9 % Percentage of total net sales 41 % 39 % Americas net sales increased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to higher net sales of iPhone, partially offset by lower net sales of iPad. Europe The following table presents Europe net sales information for the first quarter of 2017 and 2016 (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 18,521 $ 17,932 3 % Percentage of total net sales 24 % 24 % Europe net sales increased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to higher net sales of iPhone, partially offset by the effect of weakness in foreign currencies relative to the U.S. dollar and a decrease in net sales of iPad. Greater China The following table presents Greater China net sales information for the first quarter of 2017 and 2016 (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 16,233 $ 18,373 (12 )% Percentage of total net sales 21 % 24 % Greater China net sales decreased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to lower net sales of iPhone and the effect of weakness in foreign currencies relative to the U.S. dollar. 25 Japan The following table presents Japan net sales information for the first quarter of 2017 and 2016 (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 5,766 $ 4,794 20 % Percentage of total net sales 7 % 6 % Japan net sales increased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to higher net sales of iPhone and Services, and the effect of strength in the Japanese yen relative to the U.S. dollar. Rest of Asia Pacific The following table presents Rest of Asia Pacific net sales information for the first quarter of 2017 and 2016 (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Net sales $ 5,863 $ 5,448 8 % Percentage of total net sales 7 % 7 % Rest of Asia Pacific net sales increased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to higher net sales of iPhone and the effect of strength in foreign currencies relative to the U.S. dollar. Gross Margin Gross margin for the first quarter of 2017 and 2016 was as follows (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Net sales $ 78,351 $ 75,872 Cost of sales 48,175 45,449 Gross margin $ 30,176 $ 30,423 Gross margin percentage 38.5 % 40.1 % Gross margin decreased during the first quarter of 2017 compared to the same quarter in 2016 due primarily to higher product cost structures and the effect of weakness in foreign currencies relative to the U.S. dollar, partially offset by a favorable mix of products and services. The Company anticipates gross margin during the second quarter of 2017 to be between 38% and 39%. The foregoing statement regarding the Company’s expected gross margin percentage in the second quarter of 2017 is forward-looking and could differ from actual results. The Company’s future gross margins can be impacted by multiple factors including, but not limited to, those set forth in Part II, Item 1A of this Form 10-Q under the heading “Risk Factors” and those described in this paragraph. In general, the Company believes gross margins will remain under downward pressure due to a variety of factors, including continued industry-wide global product pricing pressures, increased competition, compressed product life cycles, product transitions, potential increases in the cost of components, and potential strengthening of the U.S. dollar, as well as potential increases in the costs of outside manufacturing services and a potential shift in the Company’s sales mix towards products with lower gross margins. In response to competitive pressures, the Company expects it will continue to take product pricing actions, which would adversely affect gross margins. Gross margins could also be affected by the Company’s ability to manage product quality and warranty costs effectively and to stimulate demand for certain of its products. Due to the Company’s significant international operations, its financial condition and operating results, including gross margins, could be significantly affected by fluctuations in exchange rates. 26 Operating Expenses Operating expenses for the first quarter of 2017 and 2016 were as follows (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Research and development $ 2,871 $ 2,404 Percentage of total net sales 4 % 3 % Selling, general and administrative $ 3,946 $ 3,848 Percentage of total net sales 5 % 5 % Total operating expenses $ 6,817 $ 6,252 Percentage of total net sales 9 % 8 % Research and Development The growth in R&amp;D expense during the first quarter of 2017 compared to the same quarter in 2016 was driven primarily by an increase in headcount and related expenses, and material costs to support expanded R&amp;D activities. The Company continues to believe that focused investments in R&amp;D are critical to its future growth and competitive position in the marketplace, and to the development of new and updated products that are central to the Company’s core business strategy. Selling, General and Administrative The growth in selling, general and administrative expense during the first quarter of 2017 compared to the same quarter in 2016 was driven primarily by an increase in headcount and related expenses and higher variable selling costs, partially offset by lower advertising costs. Other Income/(Expense), Net Other income/(expense), net for the first quarter of 2017 and 2016 was as follows (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Change Interest and dividend income $ 1,224 $ 941 Interest expense (525 ) (276 ) Other income/(expense), net 122 (263 ) Total other income/(expense), net $ 821 $ 402 104 % The increase in other income/(expense), net during the first quarter of 2017 compared to the same quarter in 2016 was due primarily to higher interest income and foreign exchange gains, partially offset by higher interest expense on debt. The weighted-average interest rate earned by the Company on its cash, cash equivalents and marketable securities was 1.87% and 1.65% in the first quarter of 2017 and 2016, respectively. Provision for Income Taxes Provision for income taxes and effective tax rates for the first quarter of 2017 and 2016 were as follows (dollars in millions): Three Months Ended December 31, 2016 December 26, 2015 Provision for income taxes $ 6,289 $ 6,212 Effective tax rate 26.0 % 25.3 % The Company’s effective tax rates during the first quarter of 2017 and 2016 differ from the statutory federal income tax rate of 35% due primarily to certain undistributed foreign earnings, a substantial portion of which was generated by subsidiaries organized in Ireland, for which no U.S. taxes are provided when such earnings are intended to be indefinitely reinvested outside the U.S. The higher year-over-year effective tax rate during the first quarter of 2017 was due primarily to the retroactive reinstatement of the U.S. federal R&amp;D tax credit during the first quarter of 2016. 27 The Company is subject to audits by federal, state, local and foreign tax authorities. Management believes that adequate provisions have been made for any adjustments that may result from tax examinations. However, the outcome of tax audits cannot be predicted with certainty. If any issues addressed in the Company’s tax audits are resolved in a manner not consistent with management’s expectations, the Company could be required to adjust its provision for income taxes in the period such resolution occurs. On August 30, 2016, the European Commission announced its decision that Ireland granted state aid to the Company by providing tax opinions in 1991 and 2007 concerning the tax allocation of profits of the Irish branches of two subsidiaries of the Company (the “State Aid Decision”). The State Aid Decision orders Ireland to calculate and recover additional taxes from the Company for the period June 2003 through December 2014. Irish legislative changes, effective as of January 2015, eliminated the application of the tax opinions from that date forward. The Company believes the State Aid Decision to be without merit and appealed to the General Court of the Court of Justice of the European Union. Ireland has also appealed the State Aid Decision. While the European Commission announced a recovery amount of up to €13 billion, plus interest, the actual amount of additional taxes subject to recovery is to be calculated by Ireland in accordance with the European Commission's guidance. Once the recovery amount is computed by Ireland, the Company anticipates funding it, including interest, out of foreign cash into escrow, where it will remain pending conclusion of all appeals. The Company believes that any incremental Irish corporate income taxes potentially due related to the State Aid Decision would be creditable against U.S. taxes. Recent Accounting Pronouncements Restricted Cash In November 2016, the Financial Accounting Standards Board (“FASB”) issued Accounting Standards Update (“ASU”) No. 2016-18, Statement of Cash Flows (Topic 230): Restricted Cash (“ASU 2016-18”), which enhances and clarifies the guidance on the classification and presentation of restricted cash in the statement of cash flows. The Company will adopt ASU 2016-18 in its first quarter of 2019 utilizing the retrospective adoption method. Currently, the Company's restricted cash balance is not significant. Income Taxes In October 2016, the FASB issued ASU No. 2016-16, Income Taxes (Topic 740): Intra-Entity Transfers of Assets Other Than Inventory (“ASU 2016-16”), which requires the recognition of the income tax consequences of an intra-entity transfer of an asset, other than inventory, when the transfer occurs. The Company will adopt ASU 2016-16 in its first quarter of 2019 utilizing the modified retrospective adoption method. Currently, the Company anticipates recording up to $9 billion of net deferred tax assets on its Consolidated Balance Sheets. However, the ultimate impact of adopting ASU 2016-16 will depend on the balance of intellectual property transferred between its subsidiaries as of the adoption date. The Company will recognize incremental deferred income tax expense thereafter as these deferred tax assets are utilized. Stock Compensation In March 2016, the FASB issued ASU No. 2016-09, Compensation – Stock Compensation (Topic 718): Improvements to Employee Share-Based Payment Accounting (“ASU 2016-09”), which modifies certain aspects of the accounting for share-based payment transactions, including income taxes, classification of awards, and classification in the statement of cash flows. The Company will adopt ASU 2016-09 in its first quarter of 2018. Currently, excess tax benefits or deficiencies from the Company's equity awards are recorded as additional paid-in capital in its Consolidated Balance Sheets. Upon adoption, the Company will record any excess tax benefits or deficiencies from its equity awards in its Consolidated Statements of Operations in the reporting periods in which vesting occurs. As a result, subsequent to adoption the Company's income tax expense and associated effective tax rate will be impacted by fluctuations in stock price between the grant dates and vesting dates of equity awards. Leases In February 2016, the FASB issued ASU No. 2016-02, Leases (Topic 842) (“ASU 2016-02”), which modifies lease accounting for lessees to increase transparency and comparability by recording lease assets and liabilities for operating leases and disclosing key information about leasing arrangements. ASU 2016-02 will be effective for the Company beginning in its first quarter of 2020, and early adoption is permitted. The Company will use a modified retrospective adoption approach. While the Company is currently evaluating the timing and impact of adopting ASU 2016-02, currently the Company anticipates recording lease assets and liabilities in excess of $7.5 billion on its Consolidated Balance Sheets, with no material impact to its Consolidated Statements of Operations. However, the ultimate impact of adopting ASU 2016-02 will depend on the Company's lease portfolio as of the adoption date. Financial Instruments In January 2016, the FASB issued ASU No. 2016-01, Financial Instruments – Overall (Subtopic 825-10): Recognition and Measurement of Financial Assets and Financial Liabilities (“ASU 2016-01”), which updates certain aspects of recognition, measurement, presentation and disclosure of financial instruments. The Company will adopt ASU 2016-01 in its first quarter of 2019 utilizing the modified retrospective adoption method. Based on the composition of the Company's investment portfolio, the adoption of ASU 2016-01 is not expected to have a material impact on its consolidated financial statements. 28 In June 2016, the FASB issued ASU No. 2016-13, Financial Instruments – Credit Losses (Topic 326): Measurement of Credit Losses on Financial Instruments (“ASU 2016-13”), which modifies the measurement of expected credit losses of certain financial instruments. The Company will adopt ASU 2016-13 in its first quarter of 2021 utilizing the modified retrospective adoption method. Based on the composition of the Company's investment portfolio, current market conditions, and historical credit loss activity, the adoption of ASU 2016-13 is not expected to have a material impact on its consolidated financial statements. Revenue Recognition In May 2014, the FASB issued ASU No. 2014-09, Revenue from Contracts with Customers (Topic 606) (“ASU 2014-09”), which amends the existing accounting standards for revenue recognition. ASU 2014-09 is based on principles that govern the recognition of revenue at an amount an entity expects to be entitled when products are transferred to customers. Subsequently, the FASB has issued the following standards related to ASU 2014-09: ASU No. 2016-08, Revenue from Contracts with Customers (Topic 606): Principal versus Agent Considerations (“ASU 2016-08”); ASU No. 2016-10, Revenue from Contracts with Customers (Topic 606): Identifying Performance Obligations and Licensing (“ASU 2016-10”); ASU No. 2016-12, Revenue from Contracts with Customers (Topic 606): Narrow-Scope Improvements and Practical Expedients (“ASU 2016-12”); and ASU No. 2016-20, Technical Corrections and Improvements to Topic 606, Revenue from Contracts with Customers (“ASU 2016-20”). The Company must adopt ASU 2016-08, ASU 2016-10, ASU 2016-12 and ASU 2016-20 with ASU 2014-09 (collectively, the “new revenue standards”). The new revenue standards may be applied retrospectively to each prior period presented or retrospectively with the cumulative effect recognized as of the date of adoption. The Company currently expects to adopt the new revenue standards in its first quarter of 2018 utilizing the full retrospective adoption method. The new revenue standards are not expected to have a material impact on the amount and timing of revenue recognized in the Company's consolidated financial statements. Liquidity and Capital Resources The following tables present selected financial information and statistics as of December 31, 2016 and September 24, 2016 and for the first three months of 2017 and 2016 (in millions): December 31, 2016 September 24, 2016 Cash, cash equivalents and marketable securities $ 246,090 $ 237,585 Property, plant and equipment, net $ 26,510 $ 27,010 Commercial paper $ 10,493 $ 8,105 Total term debt $ 77,056 $ 78,927 Working capital $ 19,202 $ 27,863 Three Months Ended December 31, 2016 December 26, 2015 Cash generated by operating activities $ 27,056 $ 27,463 Cash used in investing activities $ (19,122 ) $ (20,450 ) Cash used in financing activities $ (12,047 ) $ (11,444 ) The Company believes its existing balances of cash, cash equivalents and marketable securities will be sufficient to satisfy its working capital needs, capital asset purchases, outstanding commitments and other liquidity requirements associated with its existing operations over the next 12 months. The Company currently anticipates the cash used for future dividends, the share repurchase program and debt repayments will come from its current domestic cash, cash generated from on-going U.S. operating activities and from borrowings. As of December 31, 2016 and September 24, 2016, the Company’s cash, cash equivalents and marketable securities held by foreign subsidiaries were $230.2 billion and $216.0 billion, respectively, and are generally based in U.S. dollar-denominated holdings. Amounts held by foreign subsidiaries are generally subject to U.S. income taxation on repatriation to the U.S. In connection with the State Aid Decision, the European Commission announced a recovery amount of up to €13 billion, plus interest. The actual amount of additional taxes subject to recovery is to be calculated by Ireland in accordance with the European Commission's guidance. Once the recovery amount is computed by Ireland, the Company anticipates funding it, including interest, out of foreign cash into escrow, where it will remain pending conclusion of all appeals. The Company’s marketable securities investment portfolio is invested primarily in highly-rated securities, and its investment policy generally limits the amount of credit exposure to any one issuer. The policy requires investments generally to be investment grade with the objective of minimizing the potential risk of principal loss. 29 During the three months ended December 31, 2016, cash generated from operating activities of $27.1 billion was a result of $17.9 billion of net income, non-cash adjustments to net income of $5.4 billion and an increase in the net change in operating assets and liabilities of $3.7 billion. Cash used in investing activities of $19.1 billion during the three months ended December 31, 2016 consisted primarily of cash used for purchases of marketable securities, net of sales and maturities, of $15.6 billion and cash used to acquire property, plant and equipment of $3.3 billion. Cash used in financing activities of $12.0 billion during the three months ended December 31, 2016 consisted primarily of cash used to repurchase common stock of $10.9 billion and cash used to pay dividends and dividend equivalents of $3.1 billion, partially offset by a net increase in commercial paper of $2.4 billion. During the three months ended December 26, 2015, cash generated from operating activities of $27.5 billion was a result of $18.4 billion of net income, non-cash adjustments to net income of $5.7 billion and an increase in the net change in operating assets and liabilities of $3.4 billion. Cash used in investing activities of $20.5 billion during the three months ended December 26, 2015 consisted primarily of cash used for purchases of marketable securities, net of sales and maturities, of $16.1 billion and cash used to acquire property, plant and equipment of $3.6 billion. Cash used in financing activities of $11.4 billion during the three months ended December 26, 2015 consisted primarily of cash used to repurchase common stock of $6.9 billion, and cash used to pay dividends and dividend equivalents of $3.0 billion. Capital Assets The Company’s capital expenditures were $2.1 billion during the first quarter of 2017. The Company anticipates utilizing approximately $16.0 billion for capital expenditures during 2017, which includ</t>
   </si>
 </sst>
 </file>
@@ -262,7 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -280,7 +280,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
@@ -586,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="145" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,11 +597,11 @@
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="3" max="3" width="13.109375" customWidth="1"/>
     <col min="4" max="4" width="39.21875" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,11 +614,11 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -632,11 +631,11 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -649,11 +648,11 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -666,11 +665,11 @@
       <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -683,11 +682,11 @@
       <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -700,11 +699,11 @@
       <c r="D7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="E7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -717,11 +716,11 @@
       <c r="D8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="E8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -734,11 +733,11 @@
       <c r="D9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="E9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -751,11 +750,11 @@
       <c r="D10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -768,11 +767,11 @@
       <c r="D11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="E11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -785,11 +784,11 @@
       <c r="D12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="E12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -802,11 +801,11 @@
       <c r="D13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="E13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -819,11 +818,11 @@
       <c r="D14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -836,11 +835,11 @@
       <c r="D15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="E15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -853,11 +852,11 @@
       <c r="D16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="E16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -870,11 +869,11 @@
       <c r="D17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="E17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
@@ -887,11 +886,11 @@
       <c r="D18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
@@ -904,11 +903,11 @@
       <c r="D19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="E19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
@@ -921,11 +920,11 @@
       <c r="D20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="E20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
@@ -938,11 +937,11 @@
       <c r="D21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="E21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -955,11 +954,11 @@
       <c r="D22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
@@ -972,11 +971,11 @@
       <c r="D23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="E23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
@@ -989,11 +988,11 @@
       <c r="D24" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="E24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
@@ -1006,11 +1005,11 @@
       <c r="D25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -1023,11 +1022,11 @@
       <c r="D26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
@@ -1040,11 +1039,11 @@
       <c r="D27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>5</v>
       </c>
@@ -1057,11 +1056,11 @@
       <c r="D28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -1074,11 +1073,11 @@
       <c r="D29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
@@ -1091,11 +1090,11 @@
       <c r="D30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>5</v>
       </c>
@@ -1108,11 +1107,11 @@
       <c r="D31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="E31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
@@ -1125,11 +1124,11 @@
       <c r="D32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="E32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>5</v>
       </c>
@@ -1142,11 +1141,11 @@
       <c r="D33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="E33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
@@ -1159,11 +1158,11 @@
       <c r="D34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>5</v>
       </c>
@@ -1176,11 +1175,11 @@
       <c r="D35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="E35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>5</v>
       </c>
@@ -1193,11 +1192,11 @@
       <c r="D36" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="E36" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>5</v>
       </c>
@@ -1210,11 +1209,11 @@
       <c r="D37" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E37" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>6</v>
       </c>
@@ -1227,11 +1226,11 @@
       <c r="D38" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E38" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>5</v>
       </c>
@@ -1245,7 +1244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -1259,7 +1258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>5</v>
       </c>
@@ -1273,7 +1272,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>6</v>
       </c>
@@ -1287,7 +1286,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>5</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>5</v>
       </c>
@@ -1315,7 +1314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>5</v>
       </c>
@@ -1329,7 +1328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>6</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
@@ -1357,7 +1356,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>5</v>
       </c>
@@ -2165,70 +2164,70 @@
     <hyperlink ref="A36" r:id="rId34" display="https://www.sec.gov/Archives/edgar/data/320193/000162828017004790/a10-qq22017412017.htm" xr:uid="{70D76030-BEBF-40A8-B37B-02BA6BB2C1E5}"/>
     <hyperlink ref="A37" r:id="rId35" display="https://www.sec.gov/Archives/edgar/data/320193/000162828017000717/a10-qq1201712312016.htm" xr:uid="{B42F97CB-BFDE-4FD8-B759-0E6208032F49}"/>
     <hyperlink ref="A38" r:id="rId36" display="https://www.sec.gov/Archives/edgar/data/320193/000162828016020309/a201610-k9242016.htm" xr:uid="{E6CDA430-F28D-47BC-A136-0062E0347A04}"/>
-    <hyperlink ref="A39" r:id="rId37" display="https://www.sec.gov/Archives/edgar/data/320193/000162828016017809/a10-qq320166252016.htm" xr:uid="{19C3AFE5-E992-47D3-A912-77CB0280771D}"/>
-    <hyperlink ref="A40" r:id="rId38" display="https://www.sec.gov/Archives/edgar/data/320193/000119312516559625/d165350d10q.htm" xr:uid="{8E06345F-7EC6-4FCE-85A1-AF0B2A484BD9}"/>
-    <hyperlink ref="A41" r:id="rId39" display="https://www.sec.gov/Archives/edgar/data/320193/000119312516439878/d66145d10q.htm" xr:uid="{FB59C1C7-665E-415D-B246-A0397D770D0B}"/>
-    <hyperlink ref="A42" r:id="rId40" display="https://www.sec.gov/Archives/edgar/data/320193/000119312515356351/d17062d10k.htm" xr:uid="{7B44996B-E348-4F2C-B93C-1637A4A2C652}"/>
-    <hyperlink ref="A43" r:id="rId41" display="https://www.sec.gov/Archives/edgar/data/320193/000119312515259935/d927922d10q.htm" xr:uid="{1AC14539-F89D-48DA-B8EE-A32C2143679D}"/>
-    <hyperlink ref="A44" r:id="rId42" display="https://www.sec.gov/Archives/edgar/data/320193/000119312515153166/d892246d10q.htm" xr:uid="{557599B7-06EC-4BF9-82E8-D17CA783F2F9}"/>
-    <hyperlink ref="A45" r:id="rId43" display="https://www.sec.gov/Archives/edgar/data/320193/000119312515023697/d835533d10q.htm" xr:uid="{94E89346-9EC0-4F11-8F63-90A06ED29B26}"/>
-    <hyperlink ref="A46" r:id="rId44" display="https://www.sec.gov/Archives/edgar/data/320193/000119312514383437/d783162d10k.htm" xr:uid="{A84A5422-CF68-4BD4-A462-0B92FCF648A3}"/>
-    <hyperlink ref="A47" r:id="rId45" display="https://www.sec.gov/Archives/edgar/data/320193/000119312514277160/d740164d10q.htm" xr:uid="{0E4F94EB-E14E-4711-9EB0-AD13EB41C68F}"/>
-    <hyperlink ref="A48" r:id="rId46" display="https://www.sec.gov/Archives/edgar/data/320193/000119312514157311/d694710d10q.htm" xr:uid="{DB29E58E-3CD2-4999-A784-E6C185EAAE89}"/>
-    <hyperlink ref="A49" r:id="rId47" display="https://www.sec.gov/Archives/edgar/data/320193/000119312514024487/d644622d10q.htm" xr:uid="{10ED25D8-2DA9-457C-84B1-BF4F42E5BA2D}"/>
-    <hyperlink ref="A50" r:id="rId48" display="https://www.sec.gov/Archives/edgar/data/320193/000119312513416534/d590790d10k.htm" xr:uid="{62FBFC34-495D-4397-BDFA-CEA6B34C9C88}"/>
-    <hyperlink ref="A51" r:id="rId49" display="https://www.sec.gov/Archives/edgar/data/320193/000119312513300670/d552802d10q.htm" xr:uid="{9F33B2AC-7312-416D-AD5E-22B57D8F58A0}"/>
-    <hyperlink ref="A52" r:id="rId50" display="https://www.sec.gov/Archives/edgar/data/320193/000119312513168288/d501596d10q.htm" xr:uid="{62634B09-F466-4EA4-B355-823F4FEBEA21}"/>
-    <hyperlink ref="A53" r:id="rId51" display="https://www.sec.gov/Archives/edgar/data/320193/000119312513022339/d453687d10q.htm" xr:uid="{6AB47C98-F941-431F-A5AA-B10D0D0A703D}"/>
-    <hyperlink ref="A54" r:id="rId52" display="https://www.sec.gov/Archives/edgar/data/320193/000119312512444068/d411355d10k.htm" xr:uid="{4C230D25-A6AC-4618-A09B-87C5766561D6}"/>
-    <hyperlink ref="A55" r:id="rId53" display="https://www.sec.gov/Archives/edgar/data/320193/000119312512314552/d365704d10q.htm" xr:uid="{F44A9A21-BA18-4E50-BB88-DF3ECEFD6BDC}"/>
-    <hyperlink ref="A56" r:id="rId54" display="https://www.sec.gov/Archives/edgar/data/320193/000119312512182321/d297069d10q.htm" xr:uid="{7E2FFBB3-529E-4F09-A83F-B8E789C8EBBE}"/>
-    <hyperlink ref="A57" r:id="rId55" display="https://www.sec.gov/Archives/edgar/data/320193/000119312512023398/d267587d10q.htm" xr:uid="{56680A39-E2DC-4805-A7EF-D35DD6517616}"/>
-    <hyperlink ref="A58" r:id="rId56" display="https://www.sec.gov/Archives/edgar/data/320193/000119312511282113/d220209d10k.htm" xr:uid="{A189B2DC-1A42-4931-BB06-4C03A6DBBA4A}"/>
-    <hyperlink ref="A59" r:id="rId57" display="https://www.sec.gov/Archives/edgar/data/320193/000119312511192493/d10q.htm" xr:uid="{80D279A3-8D24-4D0D-969C-0326BB7482E0}"/>
-    <hyperlink ref="A60" r:id="rId58" display="https://www.sec.gov/Archives/edgar/data/320193/000119312511104388/d10q.htm" xr:uid="{08CA848E-1E1B-4447-8F9E-1DE5737BE377}"/>
-    <hyperlink ref="A61" r:id="rId59" display="https://www.sec.gov/Archives/edgar/data/320193/000119312511010144/d10q.htm" xr:uid="{B689EC45-343A-488C-A22C-A70B828BAF12}"/>
-    <hyperlink ref="A62" r:id="rId60" display="https://www.sec.gov/Archives/edgar/data/320193/000119312510238044/d10k.htm" xr:uid="{521F5AC0-A31D-4149-8C23-E6A41F417051}"/>
-    <hyperlink ref="A63" r:id="rId61" display="https://www.sec.gov/Archives/edgar/data/320193/000119312510162840/d10q.htm" xr:uid="{88D9686F-8AF8-4515-8497-5B10E82D8347}"/>
-    <hyperlink ref="A64" r:id="rId62" display="https://www.sec.gov/Archives/edgar/data/320193/000119312510088957/d10q.htm" xr:uid="{AFF423B9-D21B-459D-B9DF-99515ACA0ABC}"/>
-    <hyperlink ref="A65" r:id="rId63" display="https://www.sec.gov/Archives/edgar/data/320193/000119312510012091/d10ka.htm" xr:uid="{D1475E1A-C2C2-47A3-A01E-552182124B48}"/>
-    <hyperlink ref="A66" r:id="rId64" display="https://www.sec.gov/Archives/edgar/data/320193/000119312510012085/d10q.htm" xr:uid="{B1FA1769-8F54-4376-BFE4-BC981633972C}"/>
-    <hyperlink ref="A67" r:id="rId65" display="https://www.sec.gov/Archives/edgar/data/320193/000119312509214859/d10k.htm" xr:uid="{C457B310-689A-4BF8-8029-F9C10DAD8F5C}"/>
-    <hyperlink ref="A68" r:id="rId66" display="https://www.sec.gov/Archives/edgar/data/320193/000119312509153165/d10q.htm" xr:uid="{0E82B51A-EC6D-4FAD-A06F-57A69A366C4E}"/>
-    <hyperlink ref="A69" r:id="rId67" display="https://www.sec.gov/Archives/edgar/data/320193/000119312509087629/d10qa.htm" xr:uid="{D9AA4127-1445-4B39-811E-7B83F2B1A4FD}"/>
-    <hyperlink ref="A70" r:id="rId68" display="https://www.sec.gov/Archives/edgar/data/320193/000119312509085781/d10q.htm" xr:uid="{7FD0C19F-B60D-4E16-A267-0C50C407E706}"/>
-    <hyperlink ref="A71" r:id="rId69" display="https://www.sec.gov/Archives/edgar/data/320193/000119312509009937/d10q.htm" xr:uid="{D08C3A24-61E6-43EC-9A11-870D58FD3BFC}"/>
-    <hyperlink ref="A72" r:id="rId70" display="https://www.sec.gov/Archives/edgar/data/320193/000119312508224958/d10k.htm" xr:uid="{F9AFC983-5CAC-44D2-A47C-2342E0E4E610}"/>
-    <hyperlink ref="A73" r:id="rId71" display="https://www.sec.gov/Archives/edgar/data/320193/000119312508156421/d10q.htm" xr:uid="{E72AF849-6312-4717-ABC3-9ACB43307109}"/>
-    <hyperlink ref="A74" r:id="rId72" display="https://www.sec.gov/Archives/edgar/data/320193/000119312508097759/d10q.htm" xr:uid="{7D31D3E4-846F-4E1A-9063-42D2971E692A}"/>
-    <hyperlink ref="A75" r:id="rId73" display="https://www.sec.gov/Archives/edgar/data/320193/000119312508017426/d10q.htm" xr:uid="{BA61EDF5-A8EA-4EA7-B90D-C24755ADC184}"/>
-    <hyperlink ref="A76" r:id="rId74" display="https://www.sec.gov/Archives/edgar/data/320193/000104746907009340/a2181030z10-k.htm" xr:uid="{31B7151C-41D5-43D0-A5C6-BAFBD497BCC6}"/>
-    <hyperlink ref="A77" r:id="rId75" display="https://www.sec.gov/Archives/edgar/data/320193/000110465907059873/a07-19295_110q.htm" xr:uid="{AE1356D0-F781-421C-92DC-428BDEAA3B2D}"/>
-    <hyperlink ref="A78" r:id="rId76" display="https://www.sec.gov/Archives/edgar/data/320193/000110465907037745/a07-13266_110q.htm" xr:uid="{777EBC3D-816A-44C3-82C1-09C7476C659B}"/>
-    <hyperlink ref="A79" r:id="rId77" display="https://www.sec.gov/Archives/edgar/data/320193/000110465907006648/a07-2749_110q.htm" xr:uid="{605BB910-660D-4571-8BB2-1C0D9444E2E8}"/>
-    <hyperlink ref="A80" r:id="rId78" display="https://www.sec.gov/Archives/edgar/data/320193/000110465906084286/a06-23473_110q.htm" xr:uid="{A7B281D5-B5FB-47B1-9FB4-929A5509192A}"/>
-    <hyperlink ref="A81" r:id="rId79" display="https://www.sec.gov/Archives/edgar/data/320193/000110465906084288/a06-25759_210k.htm" xr:uid="{AD8A3F34-B325-4114-BF2A-9D83DD734CE8}"/>
-    <hyperlink ref="A82" r:id="rId80" display="https://www.sec.gov/Archives/edgar/data/320193/000110465906031303/a06-10806_110q.htm" xr:uid="{67E2B5C0-8982-4AB3-B30E-713B4893BABF}"/>
-    <hyperlink ref="A83" r:id="rId81" display="https://www.sec.gov/Archives/edgar/data/320193/000110465906005910/a06-3798_110q.htm" xr:uid="{A7097FF5-8EF9-44FB-932B-69802865F5DE}"/>
-    <hyperlink ref="A84" r:id="rId82" display="https://www.sec.gov/Archives/edgar/data/320193/000110465905058421/a05-20674_110k.htm" xr:uid="{C345894D-76C3-4D14-BE09-42E81CBFC53A}"/>
-    <hyperlink ref="A85" r:id="rId83" display="https://www.sec.gov/Archives/edgar/data/320193/000110465905035792/a05-12535_110q.htm" xr:uid="{9640E133-6E76-4878-9D53-FE437A31B517}"/>
-    <hyperlink ref="A86" r:id="rId84" display="https://www.sec.gov/Archives/edgar/data/320193/000110465905020421/a05-7551_110q.htm" xr:uid="{D0279F8B-4878-43D5-8A07-1A4A58F64F37}"/>
-    <hyperlink ref="A87" r:id="rId85" display="https://www.sec.gov/Archives/edgar/data/320193/000110465905003520/a05-2329_110q.htm" xr:uid="{7FB915EA-ECAC-4175-BE23-7E9D381E5205}"/>
-    <hyperlink ref="A88" r:id="rId86" display="https://www.sec.gov/Archives/edgar/data/320193/000104746904035975/a2147337z10-k.htm" xr:uid="{48A772F5-0925-4E03-863F-9F7DAFD9E7AC}"/>
-    <hyperlink ref="A89" r:id="rId87" display="https://www.sec.gov/Archives/edgar/data/320193/000110465904022384/a04-8198_110q.htm" xr:uid="{0064BA0E-7179-41EC-B943-58207CEA07CB}"/>
-    <hyperlink ref="A90" r:id="rId88" display="https://www.sec.gov/Archives/edgar/data/320193/000110465904013021/a04-5089_110q.htm" xr:uid="{25953D7C-7636-4B4C-BBD5-E6B2F84FAF69}"/>
-    <hyperlink ref="A91" r:id="rId89" display="https://www.sec.gov/Archives/edgar/data/320193/000110465904003080/a04-1622_110q.htm" xr:uid="{23844AD0-D9EE-4A37-89E1-1D5AC6A8E50B}"/>
-    <hyperlink ref="A92" r:id="rId90" display="https://www.sec.gov/Archives/edgar/data/320193/000104746903041604/a2124888z10-k.htm" xr:uid="{E8A0BE00-EA35-4A5F-AEDB-DF9DD5114619}"/>
-    <hyperlink ref="A93" r:id="rId91" display="https://www.sec.gov/Archives/edgar/data/320193/000110465903017766/a03-2128_110q.htm" xr:uid="{E0B50BF2-69C4-41DB-9D0D-B0301460A009}"/>
-    <hyperlink ref="A94" r:id="rId92" display="https://www.sec.gov/Archives/edgar/data/320193/000110465903009489/j0567_10q.htm" xr:uid="{D5418381-8620-4887-A956-73CF14050133}"/>
-    <hyperlink ref="A95" r:id="rId93" display="https://www.sec.gov/Archives/edgar/data/320193/000104746903004566/a2102387z10-q.htm" xr:uid="{A96E9AFB-1235-4617-AC04-37D7CDFFB0A6}"/>
-    <hyperlink ref="A96" r:id="rId94" display="https://www.sec.gov/Archives/edgar/data/320193/000104746902007674/a2096490z10-k.htm" xr:uid="{0E36728F-FA39-4536-989E-92ABBCB1532E}"/>
-    <hyperlink ref="A97" r:id="rId95" display="https://www.sec.gov/Archives/edgar/data/320193/000091205702030796/a2086025z10-q.htm" xr:uid="{F66DC20F-1639-4724-A73B-6DB1ED3BCE5C}"/>
-    <hyperlink ref="A98" r:id="rId96" display="https://www.sec.gov/Archives/edgar/data/320193/000091205702020280/a2079853z10-q.htm" xr:uid="{5E9FCDC1-C0DC-445E-97A5-3A3EC20FB299}"/>
-    <hyperlink ref="A99" r:id="rId97" display="https://www.sec.gov/Archives/edgar/data/320193/000091205702004945/a2069685z10-q.htm" xr:uid="{635398A9-EBC7-4B46-A1CD-DDA8A1DED82B}"/>
-    <hyperlink ref="A100" r:id="rId98" display="https://www.sec.gov/Archives/edgar/data/320193/000091205701528148/a2056203z10-q.htm" xr:uid="{2050E779-ABD9-405C-929F-8F2C61163563}"/>
-    <hyperlink ref="A101" r:id="rId99" display="https://www.sec.gov/Archives/edgar/data/320193/000091205701515409/a2048698z10-q.htm" xr:uid="{97B9412D-91F3-4867-BD5B-9B50390BFBE4}"/>
-    <hyperlink ref="A102" r:id="rId100" display="https://www.sec.gov/Archives/edgar/data/320193/000091205701004642/a2038036z10-q.txt" xr:uid="{8CBDA9B7-0943-41BA-B4B2-2887B52907C1}"/>
+    <hyperlink ref="A102" r:id="rId37" display="https://www.sec.gov/Archives/edgar/data/320193/000091205701004642/a2038036z10-q.txt" xr:uid="{8CBDA9B7-0943-41BA-B4B2-2887B52907C1}"/>
+    <hyperlink ref="A101" r:id="rId38" display="https://www.sec.gov/Archives/edgar/data/320193/000091205701515409/a2048698z10-q.htm" xr:uid="{97B9412D-91F3-4867-BD5B-9B50390BFBE4}"/>
+    <hyperlink ref="A100" r:id="rId39" display="https://www.sec.gov/Archives/edgar/data/320193/000091205701528148/a2056203z10-q.htm" xr:uid="{2050E779-ABD9-405C-929F-8F2C61163563}"/>
+    <hyperlink ref="A99" r:id="rId40" display="https://www.sec.gov/Archives/edgar/data/320193/000091205702004945/a2069685z10-q.htm" xr:uid="{635398A9-EBC7-4B46-A1CD-DDA8A1DED82B}"/>
+    <hyperlink ref="A98" r:id="rId41" display="https://www.sec.gov/Archives/edgar/data/320193/000091205702020280/a2079853z10-q.htm" xr:uid="{5E9FCDC1-C0DC-445E-97A5-3A3EC20FB299}"/>
+    <hyperlink ref="A97" r:id="rId42" display="https://www.sec.gov/Archives/edgar/data/320193/000091205702030796/a2086025z10-q.htm" xr:uid="{F66DC20F-1639-4724-A73B-6DB1ED3BCE5C}"/>
+    <hyperlink ref="A96" r:id="rId43" display="https://www.sec.gov/Archives/edgar/data/320193/000104746902007674/a2096490z10-k.htm" xr:uid="{0E36728F-FA39-4536-989E-92ABBCB1532E}"/>
+    <hyperlink ref="A95" r:id="rId44" display="https://www.sec.gov/Archives/edgar/data/320193/000104746903004566/a2102387z10-q.htm" xr:uid="{A96E9AFB-1235-4617-AC04-37D7CDFFB0A6}"/>
+    <hyperlink ref="A94" r:id="rId45" display="https://www.sec.gov/Archives/edgar/data/320193/000110465903009489/j0567_10q.htm" xr:uid="{D5418381-8620-4887-A956-73CF14050133}"/>
+    <hyperlink ref="A93" r:id="rId46" display="https://www.sec.gov/Archives/edgar/data/320193/000110465903017766/a03-2128_110q.htm" xr:uid="{E0B50BF2-69C4-41DB-9D0D-B0301460A009}"/>
+    <hyperlink ref="A92" r:id="rId47" display="https://www.sec.gov/Archives/edgar/data/320193/000104746903041604/a2124888z10-k.htm" xr:uid="{E8A0BE00-EA35-4A5F-AEDB-DF9DD5114619}"/>
+    <hyperlink ref="A91" r:id="rId48" display="https://www.sec.gov/Archives/edgar/data/320193/000110465904003080/a04-1622_110q.htm" xr:uid="{23844AD0-D9EE-4A37-89E1-1D5AC6A8E50B}"/>
+    <hyperlink ref="A90" r:id="rId49" display="https://www.sec.gov/Archives/edgar/data/320193/000110465904013021/a04-5089_110q.htm" xr:uid="{25953D7C-7636-4B4C-BBD5-E6B2F84FAF69}"/>
+    <hyperlink ref="A89" r:id="rId50" display="https://www.sec.gov/Archives/edgar/data/320193/000110465904022384/a04-8198_110q.htm" xr:uid="{0064BA0E-7179-41EC-B943-58207CEA07CB}"/>
+    <hyperlink ref="A88" r:id="rId51" display="https://www.sec.gov/Archives/edgar/data/320193/000104746904035975/a2147337z10-k.htm" xr:uid="{48A772F5-0925-4E03-863F-9F7DAFD9E7AC}"/>
+    <hyperlink ref="A87" r:id="rId52" display="https://www.sec.gov/Archives/edgar/data/320193/000110465905003520/a05-2329_110q.htm" xr:uid="{7FB915EA-ECAC-4175-BE23-7E9D381E5205}"/>
+    <hyperlink ref="A86" r:id="rId53" display="https://www.sec.gov/Archives/edgar/data/320193/000110465905020421/a05-7551_110q.htm" xr:uid="{D0279F8B-4878-43D5-8A07-1A4A58F64F37}"/>
+    <hyperlink ref="A85" r:id="rId54" display="https://www.sec.gov/Archives/edgar/data/320193/000110465905035792/a05-12535_110q.htm" xr:uid="{9640E133-6E76-4878-9D53-FE437A31B517}"/>
+    <hyperlink ref="A84" r:id="rId55" display="https://www.sec.gov/Archives/edgar/data/320193/000110465905058421/a05-20674_110k.htm" xr:uid="{C345894D-76C3-4D14-BE09-42E81CBFC53A}"/>
+    <hyperlink ref="A83" r:id="rId56" display="https://www.sec.gov/Archives/edgar/data/320193/000110465906005910/a06-3798_110q.htm" xr:uid="{A7097FF5-8EF9-44FB-932B-69802865F5DE}"/>
+    <hyperlink ref="A82" r:id="rId57" display="https://www.sec.gov/Archives/edgar/data/320193/000110465906031303/a06-10806_110q.htm" xr:uid="{67E2B5C0-8982-4AB3-B30E-713B4893BABF}"/>
+    <hyperlink ref="A81" r:id="rId58" display="https://www.sec.gov/Archives/edgar/data/320193/000110465906084288/a06-25759_210k.htm" xr:uid="{AD8A3F34-B325-4114-BF2A-9D83DD734CE8}"/>
+    <hyperlink ref="A80" r:id="rId59" display="https://www.sec.gov/Archives/edgar/data/320193/000110465906084286/a06-23473_110q.htm" xr:uid="{A7B281D5-B5FB-47B1-9FB4-929A5509192A}"/>
+    <hyperlink ref="A79" r:id="rId60" display="https://www.sec.gov/Archives/edgar/data/320193/000110465907006648/a07-2749_110q.htm" xr:uid="{605BB910-660D-4571-8BB2-1C0D9444E2E8}"/>
+    <hyperlink ref="A78" r:id="rId61" display="https://www.sec.gov/Archives/edgar/data/320193/000110465907037745/a07-13266_110q.htm" xr:uid="{777EBC3D-816A-44C3-82C1-09C7476C659B}"/>
+    <hyperlink ref="A77" r:id="rId62" display="https://www.sec.gov/Archives/edgar/data/320193/000110465907059873/a07-19295_110q.htm" xr:uid="{AE1356D0-F781-421C-92DC-428BDEAA3B2D}"/>
+    <hyperlink ref="A76" r:id="rId63" display="https://www.sec.gov/Archives/edgar/data/320193/000104746907009340/a2181030z10-k.htm" xr:uid="{31B7151C-41D5-43D0-A5C6-BAFBD497BCC6}"/>
+    <hyperlink ref="A75" r:id="rId64" display="https://www.sec.gov/Archives/edgar/data/320193/000119312508017426/d10q.htm" xr:uid="{BA61EDF5-A8EA-4EA7-B90D-C24755ADC184}"/>
+    <hyperlink ref="A74" r:id="rId65" display="https://www.sec.gov/Archives/edgar/data/320193/000119312508097759/d10q.htm" xr:uid="{7D31D3E4-846F-4E1A-9063-42D2971E692A}"/>
+    <hyperlink ref="A73" r:id="rId66" display="https://www.sec.gov/Archives/edgar/data/320193/000119312508156421/d10q.htm" xr:uid="{E72AF849-6312-4717-ABC3-9ACB43307109}"/>
+    <hyperlink ref="A72" r:id="rId67" display="https://www.sec.gov/Archives/edgar/data/320193/000119312508224958/d10k.htm" xr:uid="{F9AFC983-5CAC-44D2-A47C-2342E0E4E610}"/>
+    <hyperlink ref="A71" r:id="rId68" display="https://www.sec.gov/Archives/edgar/data/320193/000119312509009937/d10q.htm" xr:uid="{D08C3A24-61E6-43EC-9A11-870D58FD3BFC}"/>
+    <hyperlink ref="A70" r:id="rId69" display="https://www.sec.gov/Archives/edgar/data/320193/000119312509085781/d10q.htm" xr:uid="{7FD0C19F-B60D-4E16-A267-0C50C407E706}"/>
+    <hyperlink ref="A69" r:id="rId70" display="https://www.sec.gov/Archives/edgar/data/320193/000119312509087629/d10qa.htm" xr:uid="{D9AA4127-1445-4B39-811E-7B83F2B1A4FD}"/>
+    <hyperlink ref="A68" r:id="rId71" display="https://www.sec.gov/Archives/edgar/data/320193/000119312509153165/d10q.htm" xr:uid="{0E82B51A-EC6D-4FAD-A06F-57A69A366C4E}"/>
+    <hyperlink ref="A67" r:id="rId72" display="https://www.sec.gov/Archives/edgar/data/320193/000119312509214859/d10k.htm" xr:uid="{C457B310-689A-4BF8-8029-F9C10DAD8F5C}"/>
+    <hyperlink ref="A66" r:id="rId73" display="https://www.sec.gov/Archives/edgar/data/320193/000119312510012085/d10q.htm" xr:uid="{B1FA1769-8F54-4376-BFE4-BC981633972C}"/>
+    <hyperlink ref="A65" r:id="rId74" display="https://www.sec.gov/Archives/edgar/data/320193/000119312510012091/d10ka.htm" xr:uid="{D1475E1A-C2C2-47A3-A01E-552182124B48}"/>
+    <hyperlink ref="A64" r:id="rId75" display="https://www.sec.gov/Archives/edgar/data/320193/000119312510088957/d10q.htm" xr:uid="{AFF423B9-D21B-459D-B9DF-99515ACA0ABC}"/>
+    <hyperlink ref="A63" r:id="rId76" display="https://www.sec.gov/Archives/edgar/data/320193/000119312510162840/d10q.htm" xr:uid="{88D9686F-8AF8-4515-8497-5B10E82D8347}"/>
+    <hyperlink ref="A62" r:id="rId77" display="https://www.sec.gov/Archives/edgar/data/320193/000119312510238044/d10k.htm" xr:uid="{521F5AC0-A31D-4149-8C23-E6A41F417051}"/>
+    <hyperlink ref="A61" r:id="rId78" display="https://www.sec.gov/Archives/edgar/data/320193/000119312511010144/d10q.htm" xr:uid="{B689EC45-343A-488C-A22C-A70B828BAF12}"/>
+    <hyperlink ref="A60" r:id="rId79" display="https://www.sec.gov/Archives/edgar/data/320193/000119312511104388/d10q.htm" xr:uid="{08CA848E-1E1B-4447-8F9E-1DE5737BE377}"/>
+    <hyperlink ref="A59" r:id="rId80" display="https://www.sec.gov/Archives/edgar/data/320193/000119312511192493/d10q.htm" xr:uid="{80D279A3-8D24-4D0D-969C-0326BB7482E0}"/>
+    <hyperlink ref="A58" r:id="rId81" display="https://www.sec.gov/Archives/edgar/data/320193/000119312511282113/d220209d10k.htm" xr:uid="{A189B2DC-1A42-4931-BB06-4C03A6DBBA4A}"/>
+    <hyperlink ref="A57" r:id="rId82" display="https://www.sec.gov/Archives/edgar/data/320193/000119312512023398/d267587d10q.htm" xr:uid="{56680A39-E2DC-4805-A7EF-D35DD6517616}"/>
+    <hyperlink ref="A56" r:id="rId83" display="https://www.sec.gov/Archives/edgar/data/320193/000119312512182321/d297069d10q.htm" xr:uid="{7E2FFBB3-529E-4F09-A83F-B8E789C8EBBE}"/>
+    <hyperlink ref="A55" r:id="rId84" display="https://www.sec.gov/Archives/edgar/data/320193/000119312512314552/d365704d10q.htm" xr:uid="{F44A9A21-BA18-4E50-BB88-DF3ECEFD6BDC}"/>
+    <hyperlink ref="A54" r:id="rId85" display="https://www.sec.gov/Archives/edgar/data/320193/000119312512444068/d411355d10k.htm" xr:uid="{4C230D25-A6AC-4618-A09B-87C5766561D6}"/>
+    <hyperlink ref="A53" r:id="rId86" display="https://www.sec.gov/Archives/edgar/data/320193/000119312513022339/d453687d10q.htm" xr:uid="{6AB47C98-F941-431F-A5AA-B10D0D0A703D}"/>
+    <hyperlink ref="A52" r:id="rId87" display="https://www.sec.gov/Archives/edgar/data/320193/000119312513168288/d501596d10q.htm" xr:uid="{62634B09-F466-4EA4-B355-823F4FEBEA21}"/>
+    <hyperlink ref="A51" r:id="rId88" display="https://www.sec.gov/Archives/edgar/data/320193/000119312513300670/d552802d10q.htm" xr:uid="{9F33B2AC-7312-416D-AD5E-22B57D8F58A0}"/>
+    <hyperlink ref="A50" r:id="rId89" display="https://www.sec.gov/Archives/edgar/data/320193/000119312513416534/d590790d10k.htm" xr:uid="{62FBFC34-495D-4397-BDFA-CEA6B34C9C88}"/>
+    <hyperlink ref="A49" r:id="rId90" display="https://www.sec.gov/Archives/edgar/data/320193/000119312514024487/d644622d10q.htm" xr:uid="{10ED25D8-2DA9-457C-84B1-BF4F42E5BA2D}"/>
+    <hyperlink ref="A48" r:id="rId91" display="https://www.sec.gov/Archives/edgar/data/320193/000119312514157311/d694710d10q.htm" xr:uid="{DB29E58E-3CD2-4999-A784-E6C185EAAE89}"/>
+    <hyperlink ref="A47" r:id="rId92" display="https://www.sec.gov/Archives/edgar/data/320193/000119312514277160/d740164d10q.htm" xr:uid="{0E4F94EB-E14E-4711-9EB0-AD13EB41C68F}"/>
+    <hyperlink ref="A46" r:id="rId93" display="https://www.sec.gov/Archives/edgar/data/320193/000119312514383437/d783162d10k.htm" xr:uid="{A84A5422-CF68-4BD4-A462-0B92FCF648A3}"/>
+    <hyperlink ref="A45" r:id="rId94" display="https://www.sec.gov/Archives/edgar/data/320193/000119312515023697/d835533d10q.htm" xr:uid="{94E89346-9EC0-4F11-8F63-90A06ED29B26}"/>
+    <hyperlink ref="A44" r:id="rId95" display="https://www.sec.gov/Archives/edgar/data/320193/000119312515153166/d892246d10q.htm" xr:uid="{557599B7-06EC-4BF9-82E8-D17CA783F2F9}"/>
+    <hyperlink ref="A43" r:id="rId96" display="https://www.sec.gov/Archives/edgar/data/320193/000119312515259935/d927922d10q.htm" xr:uid="{1AC14539-F89D-48DA-B8EE-A32C2143679D}"/>
+    <hyperlink ref="A42" r:id="rId97" display="https://www.sec.gov/Archives/edgar/data/320193/000119312515356351/d17062d10k.htm" xr:uid="{7B44996B-E348-4F2C-B93C-1637A4A2C652}"/>
+    <hyperlink ref="A41" r:id="rId98" display="https://www.sec.gov/Archives/edgar/data/320193/000119312516439878/d66145d10q.htm" xr:uid="{FB59C1C7-665E-415D-B246-A0397D770D0B}"/>
+    <hyperlink ref="A40" r:id="rId99" display="https://www.sec.gov/Archives/edgar/data/320193/000119312516559625/d165350d10q.htm" xr:uid="{8E06345F-7EC6-4FCE-85A1-AF0B2A484BD9}"/>
+    <hyperlink ref="A39" r:id="rId100" display="https://www.sec.gov/Archives/edgar/data/320193/000162828016017809/a10-qq320166252016.htm" xr:uid="{19C3AFE5-E992-47D3-A912-77CB0280771D}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>